<commit_message>
- Corrections PPB et PB et mise à jour de la documentation!!!
</commit_message>
<xml_diff>
--- a/tests/output_test_data/mp_global_projection_reporting.xlsx
+++ b/tests/output_test_data/mp_global_projection_reporting.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef77bd1ebbbb3aed/Modele_ALM/tests/output_test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_FFC65FC05B79ECDE962EABFC8A2F55C961B401BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4628842-15A6-964A-9B3F-4200153F728A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6700" yWindow="1520" windowWidth="23860" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" calcCompleted="0"/>
 </workbook>
 </file>
 
@@ -97,8 +103,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,10 +156,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -161,11 +176,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -207,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +262,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,6 +314,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,61 +507,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.6640625" style="4" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
     </row>
-    <row r="2" spans="1:42">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -629,8 +693,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -757,8 +821,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -885,8 +949,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -1013,520 +1077,520 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>426333.403789871</v>
+        <v>43518.266528369917</v>
       </c>
       <c r="D7">
-        <v>412979.4449012851</v>
+        <v>43418.11064879295</v>
       </c>
       <c r="E7">
-        <v>400755.0331838224</v>
+        <v>43429.354720710689</v>
       </c>
       <c r="F7">
-        <v>389396.3150546101</v>
+        <v>43524.93153912251</v>
       </c>
       <c r="G7">
-        <v>378601.9054764328</v>
+        <v>43666.16642959146</v>
       </c>
       <c r="H7">
-        <v>368239.9178891573</v>
+        <v>43832.473282778687</v>
       </c>
       <c r="I7">
-        <v>358180.3375621123</v>
+        <v>44009.973621243313</v>
       </c>
       <c r="J7">
-        <v>348003.7446590445</v>
+        <v>44150.992552086253</v>
       </c>
       <c r="K7">
-        <v>337968.864532123</v>
+        <v>44276.491336901257</v>
       </c>
       <c r="L7">
-        <v>328035.3793706441</v>
+        <v>44353.918951318206</v>
       </c>
       <c r="M7">
-        <v>318321.1048080911</v>
+        <v>44392.622001896038</v>
       </c>
       <c r="N7">
-        <v>308646.6496605732</v>
+        <v>44368.166259867037</v>
       </c>
       <c r="O7">
-        <v>299059.1051055221</v>
+        <v>44273.204296472257</v>
       </c>
       <c r="P7">
-        <v>289288.0295661353</v>
+        <v>44086.020948839949</v>
       </c>
       <c r="Q7">
-        <v>279238.1225030811</v>
+        <v>43795.060448787794</v>
       </c>
       <c r="R7">
-        <v>268794.0247489549</v>
+        <v>43399.583817342187</v>
       </c>
       <c r="S7">
-        <v>258125.9839387729</v>
+        <v>42936.552075322099</v>
       </c>
       <c r="T7">
-        <v>247655.9833447855</v>
+        <v>42465.015671323978</v>
       </c>
       <c r="U7">
-        <v>237393.2566051571</v>
+        <v>41965.91719964247</v>
       </c>
       <c r="V7">
-        <v>227303.8630076209</v>
+        <v>41401.314731858532</v>
       </c>
       <c r="W7">
-        <v>217569.4888679688</v>
+        <v>40779.52969886014</v>
       </c>
       <c r="X7">
-        <v>208153.8958868035</v>
+        <v>40025.36336445839</v>
       </c>
       <c r="Y7">
-        <v>199299.4375118793</v>
+        <v>39235.834054352817</v>
       </c>
       <c r="Z7">
-        <v>191068.9493478254</v>
+        <v>38463.688802030963</v>
       </c>
       <c r="AA7">
-        <v>183479.5084372984</v>
+        <v>37768.983599308507</v>
       </c>
       <c r="AB7">
-        <v>176558.9093418652</v>
+        <v>37186.46938146621</v>
       </c>
       <c r="AC7">
-        <v>170171.1677138339</v>
+        <v>36691.065552478853</v>
       </c>
       <c r="AD7">
-        <v>164331.101640833</v>
+        <v>36272.666129374178</v>
       </c>
       <c r="AE7">
-        <v>158920.3182913687</v>
+        <v>35897.548614317537</v>
       </c>
       <c r="AF7">
-        <v>153861.8078300868</v>
+        <v>35540.884833702134</v>
       </c>
       <c r="AG7">
-        <v>149024.6360014745</v>
+        <v>35140.434881312452</v>
       </c>
       <c r="AH7">
-        <v>144183.194925903</v>
+        <v>34590.101311198523</v>
       </c>
       <c r="AI7">
-        <v>139399.3171706788</v>
+        <v>33490.530299685961</v>
       </c>
       <c r="AJ7">
-        <v>134751.2775325517</v>
+        <v>32056.16063937057</v>
       </c>
       <c r="AK7">
-        <v>130034.7906630503</v>
+        <v>30430.900550146729</v>
       </c>
       <c r="AL7">
-        <v>125453.2755975306</v>
+        <v>28864.853107317718</v>
       </c>
       <c r="AM7">
-        <v>121067.6111674424</v>
+        <v>27527.7462852235</v>
       </c>
       <c r="AN7">
-        <v>116847.5016952787</v>
+        <v>26433.02651942318</v>
       </c>
       <c r="AO7">
-        <v>112498.6962968419</v>
+        <v>25497.798078377989</v>
       </c>
       <c r="AP7">
-        <v>108072.0527842961</v>
+        <v>24611.225583912928</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>17560.43782871425</v>
+        <v>18236.888884505959</v>
       </c>
       <c r="D8">
-        <v>16181.15322003988</v>
+        <v>16994.14413989905</v>
       </c>
       <c r="E8">
-        <v>15094.44191065215</v>
+        <v>16009.235326458889</v>
       </c>
       <c r="F8">
-        <v>14228.67772952445</v>
+        <v>15270.85137769514</v>
       </c>
       <c r="G8">
-        <v>13627.9625476493</v>
+        <v>14863.548755779209</v>
       </c>
       <c r="H8">
-        <v>13233.1839289991</v>
+        <v>14726.12125210565</v>
       </c>
       <c r="I8">
-        <v>13011.70577805768</v>
+        <v>14787.972862989751</v>
       </c>
       <c r="J8">
-        <v>12983.89093539645</v>
+        <v>15097.06756309861</v>
       </c>
       <c r="K8">
-        <v>12666.95786134237</v>
+        <v>15162.878327500401</v>
       </c>
       <c r="L8">
-        <v>12323.40685227728</v>
+        <v>15538.41944917006</v>
       </c>
       <c r="M8">
-        <v>11869.81002171237</v>
+        <v>15711.92895460111</v>
       </c>
       <c r="N8">
-        <v>11745.32547878231</v>
+        <v>16188.19762194252</v>
       </c>
       <c r="O8">
-        <v>11691.89463952578</v>
+        <v>16829.63060536531</v>
       </c>
       <c r="P8">
-        <v>12197.5089494357</v>
+        <v>18025.966742868441</v>
       </c>
       <c r="Q8">
-        <v>12374.00847934712</v>
+        <v>18700.592634724049</v>
       </c>
       <c r="R8">
-        <v>12552.86842528497</v>
+        <v>19259.569973970301</v>
       </c>
       <c r="S8">
-        <v>12423.77816956886</v>
+        <v>19250.73810375739</v>
       </c>
       <c r="T8">
-        <v>11870.11773559374</v>
+        <v>18636.276017775181</v>
       </c>
       <c r="U8">
-        <v>11308.33852561303</v>
+        <v>18109.843180915821</v>
       </c>
       <c r="V8">
-        <v>10979.6318712126</v>
+        <v>18074.362159489028</v>
       </c>
       <c r="W8">
-        <v>10520.24883865171</v>
+        <v>18023.53590584937</v>
       </c>
       <c r="X8">
-        <v>10168.40637441165</v>
+        <v>19034.031066505639</v>
       </c>
       <c r="Y8">
-        <v>9609.456060753559</v>
+        <v>19110.46764097819</v>
       </c>
       <c r="Z8">
-        <v>9018.636983394619</v>
+        <v>18758.285343178432</v>
       </c>
       <c r="AA8">
-        <v>8397.121998019544</v>
+        <v>17766.954299609049</v>
       </c>
       <c r="AB8">
-        <v>7772.736376780347</v>
+        <v>16436.306062423519</v>
       </c>
       <c r="AC8">
-        <v>7308.615876361291</v>
+        <v>15413.583530954509</v>
       </c>
       <c r="AD8">
-        <v>6842.308564739925</v>
+        <v>14572.188833600891</v>
       </c>
       <c r="AE8">
-        <v>6566.224805584632</v>
+        <v>14252.835137839829</v>
       </c>
       <c r="AF8">
-        <v>6285.59978291093</v>
+        <v>14060.72493416512</v>
       </c>
       <c r="AG8">
-        <v>6047.95624824172</v>
+        <v>14209.58798648576</v>
       </c>
       <c r="AH8">
-        <v>6035.01479937639</v>
+        <v>15243.298575986981</v>
       </c>
       <c r="AI8">
-        <v>5874.953212421167</v>
+        <v>19102.38802984446</v>
       </c>
       <c r="AJ8">
-        <v>5650.813337883128</v>
+        <v>21160.632329690819</v>
       </c>
       <c r="AK8">
-        <v>5486.969218179765</v>
+        <v>22023.65621389763</v>
       </c>
       <c r="AL8">
-        <v>5220.050816389809</v>
+        <v>20927.805100093239</v>
       </c>
       <c r="AM8">
-        <v>4949.175223081577</v>
+        <v>18544.884646917861</v>
       </c>
       <c r="AN8">
-        <v>4787.246729744676</v>
+        <v>16115.450071526609</v>
       </c>
       <c r="AO8">
-        <v>4967.422447698244</v>
+        <v>14365.91208553238</v>
       </c>
       <c r="AP8">
-        <v>5070.914220802742</v>
+        <v>13517.42367905319</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>663782.8734332257</v>
+        <v>692067.61839274841</v>
       </c>
       <c r="D9">
-        <v>621572.2261375544</v>
+        <v>652965.9982048251</v>
       </c>
       <c r="E9">
-        <v>590294.1542723742</v>
+        <v>624475.39044221235</v>
       </c>
       <c r="F9">
-        <v>565522.4677526159</v>
+        <v>603980.58127964265</v>
       </c>
       <c r="G9">
-        <v>549904.5330558221</v>
+        <v>596065.32379051135</v>
       </c>
       <c r="H9">
-        <v>540057.2806877651</v>
+        <v>596999.76485372894</v>
       </c>
       <c r="I9">
-        <v>535975.5298240231</v>
+        <v>604863.63765360159</v>
       </c>
       <c r="J9">
-        <v>539175.0502756309</v>
+        <v>621773.80204239243</v>
       </c>
       <c r="K9">
-        <v>532721.564430445</v>
+        <v>631279.05442036584</v>
       </c>
       <c r="L9">
-        <v>524690.6800954051</v>
+        <v>648017.79567084811</v>
       </c>
       <c r="M9">
-        <v>514405.5846228595</v>
+        <v>661037.64804282307</v>
       </c>
       <c r="N9">
-        <v>510734.4276705485</v>
+        <v>679504.01688370423</v>
       </c>
       <c r="O9">
-        <v>509768.1144785301</v>
+        <v>702448.32011735975</v>
       </c>
       <c r="P9">
-        <v>518942.3948085235</v>
+        <v>742739.96515234304</v>
       </c>
       <c r="Q9">
-        <v>526380.3733923687</v>
+        <v>778052.04695131746</v>
       </c>
       <c r="R9">
-        <v>537711.3959032474</v>
+        <v>814758.22578941646</v>
       </c>
       <c r="S9">
-        <v>545596.9433307982</v>
+        <v>839754.09391442104</v>
       </c>
       <c r="T9">
-        <v>536583.9985799734</v>
+        <v>838936.78087834269</v>
       </c>
       <c r="U9">
-        <v>524193.1683637636</v>
+        <v>836983.37654471945</v>
       </c>
       <c r="V9">
-        <v>512826.0379666231</v>
+        <v>844487.37590033188</v>
       </c>
       <c r="W9">
-        <v>495809.6678427169</v>
+        <v>849904.66100712225</v>
       </c>
       <c r="X9">
-        <v>487804.6694843319</v>
+        <v>888585.14652144071</v>
       </c>
       <c r="Y9">
-        <v>470360.0582653616</v>
+        <v>897050.01761251083</v>
       </c>
       <c r="Z9">
-        <v>450644.5209794272</v>
+        <v>890063.1378152417</v>
       </c>
       <c r="AA9">
-        <v>427370.0499374114</v>
+        <v>862349.63051614189</v>
       </c>
       <c r="AB9">
-        <v>399925.7440779393</v>
+        <v>819769.75508785388</v>
       </c>
       <c r="AC9">
-        <v>374708.0872475833</v>
+        <v>781431.88989497756</v>
       </c>
       <c r="AD9">
-        <v>350147.2025973919</v>
+        <v>748271.93366428697</v>
       </c>
       <c r="AE9">
-        <v>331915.4784441273</v>
+        <v>729571.23230321577</v>
       </c>
       <c r="AF9">
-        <v>317035.0404210881</v>
+        <v>719864.55760604877</v>
       </c>
       <c r="AG9">
-        <v>306360.38495148</v>
+        <v>725858.87282712781</v>
       </c>
       <c r="AH9">
-        <v>303250.8058746445</v>
+        <v>760855.47738972504</v>
       </c>
       <c r="AI9">
-        <v>296409.2365218955</v>
+        <v>887475.92735273985</v>
       </c>
       <c r="AJ9">
-        <v>287957.1463219552</v>
+        <v>951045.21447156824</v>
       </c>
       <c r="AK9">
-        <v>288047.9326210024</v>
+        <v>973166.57693948376</v>
       </c>
       <c r="AL9">
-        <v>282057.5114978813</v>
+        <v>930765.25278711761</v>
       </c>
       <c r="AM9">
-        <v>274032.265006659</v>
+        <v>848249.964277972</v>
       </c>
       <c r="AN9">
-        <v>266185.2571489883</v>
+        <v>766836.75929602585</v>
       </c>
       <c r="AO9">
-        <v>262614.8322997764</v>
+        <v>709743.68372374203</v>
       </c>
       <c r="AP9">
-        <v>258261.1821921998</v>
+        <v>683540.65340311592</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>65707.94508724248</v>
+        <v>60078.447224256808</v>
       </c>
       <c r="D10">
-        <v>67947.223125196</v>
+        <v>63271.306967338809</v>
       </c>
       <c r="E10">
-        <v>70493.44574194516</v>
+        <v>66988.616654839934</v>
       </c>
       <c r="F10">
-        <v>73299.17797991405</v>
+        <v>71263.104066607862</v>
       </c>
       <c r="G10">
-        <v>76312.65464752013</v>
+        <v>76081.635828863029</v>
       </c>
       <c r="H10">
-        <v>79481.24948472228</v>
+        <v>81380.876380341608</v>
       </c>
       <c r="I10">
-        <v>82757.1450462059</v>
+        <v>87117.649889090113</v>
       </c>
       <c r="J10">
-        <v>86094.06192375423</v>
+        <v>93283.01354195163</v>
       </c>
       <c r="K10">
-        <v>89510.03759273353</v>
+        <v>99883.216452721143</v>
       </c>
       <c r="L10">
-        <v>93019.60795087591</v>
+        <v>106857.7911642737</v>
       </c>
       <c r="M10">
-        <v>96598.58590322077</v>
+        <v>114199.8131248892</v>
       </c>
       <c r="N10">
-        <v>100182.4046203431</v>
+        <v>121790.3767715532</v>
       </c>
       <c r="O10">
-        <v>103716.3766837806</v>
+        <v>129592.59724021101</v>
       </c>
       <c r="P10">
-        <v>107060.3322824452</v>
+        <v>137512.99345342189</v>
       </c>
       <c r="Q10">
-        <v>110088.821528192</v>
+        <v>145585.05046305171</v>
       </c>
       <c r="R10">
-        <v>112614.59521251</v>
+        <v>153784.59802463351</v>
       </c>
       <c r="S10">
-        <v>114566.4357541598</v>
+        <v>162068.23167367341</v>
       </c>
       <c r="T10">
-        <v>115982.4439341648</v>
+        <v>170638.0256319477</v>
       </c>
       <c r="U10">
-        <v>116871.5880198305</v>
+        <v>179492.128764503</v>
       </c>
       <c r="V10">
-        <v>117231.3724924482</v>
+        <v>188660.45333578839</v>
       </c>
       <c r="W10">
-        <v>117028.3227368372</v>
+        <v>197881.85065221961</v>
       </c>
       <c r="X10">
-        <v>116206.680554838</v>
+        <v>206693.9728184772</v>
       </c>
       <c r="Y10">
-        <v>114772.7517873</v>
+        <v>214808.27879314471</v>
       </c>
       <c r="Z10">
-        <v>112837.4346293902</v>
+        <v>221974.384325472</v>
       </c>
       <c r="AA10">
-        <v>110486.1529953032</v>
+        <v>228246.5804009219</v>
       </c>
       <c r="AB10">
-        <v>107844.6353977459</v>
+        <v>233616.1753916525</v>
       </c>
       <c r="AC10">
-        <v>105004.0242957475</v>
+        <v>237949.4434944794</v>
       </c>
       <c r="AD10">
-        <v>102007.0476710918</v>
+        <v>241027.0402085621</v>
       </c>
       <c r="AE10">
-        <v>98891.35248353292</v>
+        <v>242659.11365682489</v>
       </c>
       <c r="AF10">
-        <v>95725.91580647121</v>
+        <v>242904.542682536</v>
       </c>
       <c r="AG10">
-        <v>92586.61957552032</v>
+        <v>241989.6530546275</v>
       </c>
       <c r="AH10">
-        <v>89564.65116546776</v>
+        <v>240059.99822815479</v>
       </c>
       <c r="AI10">
-        <v>86757.03560541694</v>
+        <v>237007.52599080201</v>
       </c>
       <c r="AJ10">
-        <v>84247.68193580436</v>
+        <v>233203.59523136151</v>
       </c>
       <c r="AK10">
-        <v>82032.77380944225</v>
+        <v>229158.75958892429</v>
       </c>
       <c r="AL10">
-        <v>80195.94461078974</v>
+        <v>225645.42531574689</v>
       </c>
       <c r="AM10">
-        <v>78739.69935153237</v>
+        <v>223166.9897175502</v>
       </c>
       <c r="AN10">
-        <v>77661.46203964781</v>
+        <v>221982.40883578151</v>
       </c>
       <c r="AO10">
-        <v>76887.29617275926</v>
+        <v>222193.70535131681</v>
       </c>
       <c r="AP10">
-        <v>76345.36549072753</v>
+        <v>223612.96669978549</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1653,264 +1717,264 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>33925.06358355082</v>
+        <v>33854.174498439228</v>
       </c>
       <c r="D12">
-        <v>32962.39971219559</v>
+        <v>33729.787051337044</v>
       </c>
       <c r="E12">
-        <v>32074.47230715554</v>
+        <v>33683.090541003483</v>
       </c>
       <c r="F12">
-        <v>31246.16778254386</v>
+        <v>33698.4555038201</v>
       </c>
       <c r="G12">
-        <v>30455.20763640739</v>
+        <v>33747.662697761531</v>
       </c>
       <c r="H12">
-        <v>29687.17510450047</v>
+        <v>33810.191015493088</v>
       </c>
       <c r="I12">
-        <v>28927.3856648611</v>
+        <v>33869.393890919368</v>
       </c>
       <c r="J12">
-        <v>28156.37029212223</v>
+        <v>33901.923284734599</v>
       </c>
       <c r="K12">
-        <v>27396.96846844056</v>
+        <v>33924.443773028746</v>
       </c>
       <c r="L12">
-        <v>26652.52966541433</v>
+        <v>33918.021412439368</v>
       </c>
       <c r="M12">
-        <v>25928.67696183769</v>
+        <v>33890.560511251897</v>
       </c>
       <c r="N12">
-        <v>25209.39344996382</v>
+        <v>33827.931453727957</v>
       </c>
       <c r="O12">
-        <v>24488.61470201133</v>
+        <v>33718.479518241977</v>
       </c>
       <c r="P12">
-        <v>23740.81708476292</v>
+        <v>33516.794455014111</v>
       </c>
       <c r="Q12">
-        <v>22969.35690708615</v>
+        <v>33231.033166153589</v>
       </c>
       <c r="R12">
-        <v>22163.17998637616</v>
+        <v>32853.003768302413</v>
       </c>
       <c r="S12">
-        <v>21328.00354047658</v>
+        <v>32405.145087910561</v>
       </c>
       <c r="T12">
-        <v>20503.06274357161</v>
+        <v>31946.32697747073</v>
       </c>
       <c r="U12">
-        <v>19695.34948727239</v>
+        <v>31477.229160031438</v>
       </c>
       <c r="V12">
-        <v>18902.04397781501</v>
+        <v>30973.294684998331</v>
       </c>
       <c r="W12">
-        <v>18137.85309747683</v>
+        <v>30438.887028000849</v>
       </c>
       <c r="X12">
-        <v>17381.29641602237</v>
+        <v>29790.455861596751</v>
       </c>
       <c r="Y12">
-        <v>16655.2756048857</v>
+        <v>29098.674981660792</v>
       </c>
       <c r="Z12">
-        <v>15965.13225658712</v>
+        <v>28399.917048887051</v>
       </c>
       <c r="AA12">
-        <v>15319.21862174088</v>
+        <v>27744.861739827302</v>
       </c>
       <c r="AB12">
-        <v>14728.23282894258</v>
+        <v>27172.278617038941</v>
       </c>
       <c r="AC12">
-        <v>14187.74789229343</v>
+        <v>26675.37564392047</v>
       </c>
       <c r="AD12">
-        <v>13697.74536332039</v>
+        <v>26245.219711169349</v>
       </c>
       <c r="AE12">
-        <v>13244.05676536705</v>
+        <v>25849.478048045112</v>
       </c>
       <c r="AF12">
-        <v>12819.6205916456</v>
+        <v>25468.273172803849</v>
       </c>
       <c r="AG12">
-        <v>12414.83724254153</v>
+        <v>25063.70775467428</v>
       </c>
       <c r="AH12">
-        <v>12011.29710884133</v>
+        <v>24562.04078295052</v>
       </c>
       <c r="AI12">
-        <v>11618.3915984597</v>
+        <v>23728.05235278896</v>
       </c>
       <c r="AJ12">
-        <v>11240.43342552376</v>
+        <v>22698.36419969421</v>
       </c>
       <c r="AK12">
-        <v>10856.1993911132</v>
+        <v>21563.351908936202</v>
       </c>
       <c r="AL12">
-        <v>10480.03869531846</v>
+        <v>20476.456332472819</v>
       </c>
       <c r="AM12">
-        <v>10116.58703974101</v>
+        <v>19539.643005934839</v>
       </c>
       <c r="AN12">
-        <v>9765.139908967913</v>
+        <v>18758.410625162309</v>
       </c>
       <c r="AO12">
-        <v>9415.057326607246</v>
+        <v>18080.829588959448</v>
       </c>
       <c r="AP12">
-        <v>9068.08964610705</v>
+        <v>17435.3977308209</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>564149.864762433</v>
+        <v>598134.99667005229</v>
       </c>
       <c r="D13">
-        <v>520662.6033001625</v>
+        <v>555964.90418614924</v>
       </c>
       <c r="E13">
-        <v>487726.2362232734</v>
+        <v>523803.68324636889</v>
       </c>
       <c r="F13">
-        <v>460977.1219901577</v>
+        <v>499019.02170921472</v>
       </c>
       <c r="G13">
-        <v>443136.6707718947</v>
+        <v>486236.02526388672</v>
       </c>
       <c r="H13">
-        <v>430888.8560985424</v>
+        <v>481808.69745789422</v>
       </c>
       <c r="I13">
-        <v>424290.9991129561</v>
+        <v>483876.59387359209</v>
       </c>
       <c r="J13">
-        <v>424924.6180597545</v>
+        <v>494588.86521570617</v>
       </c>
       <c r="K13">
-        <v>415814.5583692708</v>
+        <v>497471.39419461589</v>
       </c>
       <c r="L13">
-        <v>405018.542479115</v>
+        <v>507241.98309413512</v>
       </c>
       <c r="M13">
-        <v>391878.3217578011</v>
+        <v>512947.27440668189</v>
       </c>
       <c r="N13">
-        <v>385342.6296002416</v>
+        <v>523885.70865842298</v>
       </c>
       <c r="O13">
-        <v>381563.1230927382</v>
+        <v>539137.24335890682</v>
       </c>
       <c r="P13">
-        <v>388141.2454413155</v>
+        <v>571710.177243907</v>
       </c>
       <c r="Q13">
-        <v>393322.1949570905</v>
+        <v>599235.96332211222</v>
       </c>
       <c r="R13">
-        <v>402933.6207043614</v>
+        <v>628120.62399648048</v>
       </c>
       <c r="S13">
-        <v>409702.5040361616</v>
+        <v>645280.71715283708</v>
       </c>
       <c r="T13">
-        <v>400098.4919022371</v>
+        <v>636352.42826892424</v>
       </c>
       <c r="U13">
-        <v>387626.2308566608</v>
+        <v>626014.01862018497</v>
       </c>
       <c r="V13">
-        <v>376692.62149636</v>
+        <v>624853.62787954521</v>
       </c>
       <c r="W13">
-        <v>360643.4920084031</v>
+        <v>621583.92332690186</v>
       </c>
       <c r="X13">
-        <v>354216.6925134717</v>
+        <v>652100.71784136677</v>
       </c>
       <c r="Y13">
-        <v>338932.0308731759</v>
+        <v>653143.06383770541</v>
       </c>
       <c r="Z13">
-        <v>321841.9540934496</v>
+        <v>639688.83644088265</v>
       </c>
       <c r="AA13">
-        <v>301564.6783203675</v>
+        <v>606358.1883753927</v>
       </c>
       <c r="AB13">
-        <v>277352.8758512508</v>
+        <v>558981.3010791624</v>
       </c>
       <c r="AC13">
-        <v>255516.3150595426</v>
+        <v>516807.07075657771</v>
       </c>
       <c r="AD13">
-        <v>234442.4095629796</v>
+        <v>480999.6737445555</v>
       </c>
       <c r="AE13">
-        <v>219780.0691952273</v>
+        <v>461062.64059834578</v>
       </c>
       <c r="AF13">
-        <v>208489.5040229714</v>
+        <v>451491.74175070901</v>
       </c>
       <c r="AG13">
-        <v>201358.9281334183</v>
+        <v>458805.51201782603</v>
       </c>
       <c r="AH13">
-        <v>201674.8576003354</v>
+        <v>496233.43837861973</v>
       </c>
       <c r="AI13">
-        <v>198033.8093180188</v>
+        <v>626740.34900914889</v>
       </c>
       <c r="AJ13">
-        <v>192469.030960627</v>
+        <v>695143.25504051254</v>
       </c>
       <c r="AK13">
-        <v>195158.9594204469</v>
+        <v>722444.46544162324</v>
       </c>
       <c r="AL13">
-        <v>191381.528191773</v>
+        <v>684643.37113889796</v>
       </c>
       <c r="AM13">
-        <v>185175.9786153857</v>
+        <v>605543.33155448688</v>
       </c>
       <c r="AN13">
-        <v>178758.6552003726</v>
+        <v>526095.93983508216</v>
       </c>
       <c r="AO13">
-        <v>176312.4788004099</v>
+        <v>469469.14878346567</v>
       </c>
       <c r="AP13">
-        <v>172847.7270553653</v>
+        <v>442492.28897250962</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -2037,8 +2101,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -2165,8 +2229,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -2293,8 +2357,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -2421,8 +2485,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -2549,8 +2613,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:42">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19">
@@ -2677,392 +2741,392 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:42">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>13837.34716937473</v>
+        <v>31749.302369869401</v>
       </c>
       <c r="D20">
-        <v>13688.00030169149</v>
+        <v>31881.4818103709</v>
       </c>
       <c r="E20">
-        <v>13568.56513852728</v>
+        <v>32106.270836790631</v>
       </c>
       <c r="F20">
-        <v>13467.75813430705</v>
+        <v>32400.53035843961</v>
       </c>
       <c r="G20">
-        <v>13372.30354794464</v>
+        <v>32729.609746647471</v>
       </c>
       <c r="H20">
-        <v>13275.86214228611</v>
+        <v>33073.813094092278</v>
       </c>
       <c r="I20">
-        <v>13157.21011982694</v>
+        <v>33403.8165239031</v>
       </c>
       <c r="J20">
-        <v>13012.80639879324</v>
+        <v>33694.028813712277</v>
       </c>
       <c r="K20">
-        <v>12857.9795218356</v>
+        <v>33967.326803822289</v>
       </c>
       <c r="L20">
-        <v>12704.07151136514</v>
+        <v>34210.87975511339</v>
       </c>
       <c r="M20">
-        <v>12563.4001866323</v>
+        <v>34444.375937594377</v>
       </c>
       <c r="N20">
-        <v>12437.04080377654</v>
+        <v>34668.822335900382</v>
       </c>
       <c r="O20">
-        <v>12308.64501945086</v>
+        <v>34852.67680313965</v>
       </c>
       <c r="P20">
-        <v>12159.67267306486</v>
+        <v>34945.7508856985</v>
       </c>
       <c r="Q20">
-        <v>11979.67383816421</v>
+        <v>34940.179106597207</v>
       </c>
       <c r="R20">
-        <v>11738.90858722928</v>
+        <v>34789.478611010811</v>
       </c>
       <c r="S20">
-        <v>11434.91902103561</v>
+        <v>34516.433997460401</v>
       </c>
       <c r="T20">
-        <v>11104.03898564428</v>
+        <v>34197.84586104042</v>
       </c>
       <c r="U20">
-        <v>10772.31693735847</v>
+        <v>33861.305524496718</v>
       </c>
       <c r="V20">
-        <v>10454.54283532805</v>
+        <v>33506.57500378738</v>
       </c>
       <c r="W20">
-        <v>10159.82349925018</v>
+        <v>33147.997440042913</v>
       </c>
       <c r="X20">
-        <v>9850.222498590399</v>
+        <v>32683.299825988772</v>
       </c>
       <c r="Y20">
-        <v>9535.261725396014</v>
+        <v>32169.183204697048</v>
       </c>
       <c r="Z20">
-        <v>9211.718442958361</v>
+        <v>31628.455366061691</v>
       </c>
       <c r="AA20">
-        <v>8897.29775006634</v>
+        <v>31119.432391181021</v>
       </c>
       <c r="AB20">
-        <v>8610.565757172188</v>
+        <v>30691.02146622034</v>
       </c>
       <c r="AC20">
-        <v>8360.507563211542</v>
+        <v>30347.522815020169</v>
       </c>
       <c r="AD20">
-        <v>8147.595439080023</v>
+        <v>30086.043344383019</v>
       </c>
       <c r="AE20">
-        <v>7963.736589737643</v>
+        <v>29880.520534954288</v>
       </c>
       <c r="AF20">
-        <v>7799.589250896084</v>
+        <v>29705.532915951211</v>
       </c>
       <c r="AG20">
-        <v>7647.37782901172</v>
+        <v>29508.432453130161</v>
       </c>
       <c r="AH20">
-        <v>7496.878989218442</v>
+        <v>29194.025573051429</v>
       </c>
       <c r="AI20">
-        <v>7353.347815610935</v>
+        <v>28430.206731181559</v>
       </c>
       <c r="AJ20">
-        <v>7215.014192837861</v>
+        <v>27382.80492351174</v>
       </c>
       <c r="AK20">
-        <v>7058.585991718755</v>
+        <v>26161.722294927851</v>
       </c>
       <c r="AL20">
-        <v>6893.128217451352</v>
+        <v>24970.640337299061</v>
       </c>
       <c r="AM20">
-        <v>6722.934934191042</v>
+        <v>23953.020037936789</v>
       </c>
       <c r="AN20">
-        <v>6555.142107729608</v>
+        <v>23124.872526669511</v>
       </c>
       <c r="AO20">
-        <v>6383.627836040776</v>
+        <v>22420.962389044071</v>
       </c>
       <c r="AP20">
-        <v>6209.215445071212</v>
+        <v>21747.114265946249</v>
       </c>
     </row>
-    <row r="21" spans="1:42">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>4.415549144016001</v>
+        <v>4.5399996391239981</v>
       </c>
       <c r="D21">
-        <v>4.102649747315472</v>
+        <v>4.155664675437265</v>
       </c>
       <c r="E21">
-        <v>3.853589491191904</v>
+        <v>3.8401416974020601</v>
       </c>
       <c r="F21">
-        <v>3.634811228366353</v>
+        <v>3.566986720682134</v>
       </c>
       <c r="G21">
-        <v>3.477765630378583</v>
+        <v>3.376883871816323</v>
       </c>
       <c r="H21">
-        <v>3.345655706830422</v>
+        <v>3.2310934841529142</v>
       </c>
       <c r="I21">
-        <v>3.235470483355613</v>
+        <v>3.1148411955517288</v>
       </c>
       <c r="J21">
-        <v>3.157922713540279</v>
+        <v>3.0331001301289779</v>
       </c>
       <c r="K21">
-        <v>3.047887485178672</v>
+        <v>2.945446165009586</v>
       </c>
       <c r="L21">
-        <v>2.973910013950666</v>
+        <v>2.9644827415566959</v>
       </c>
       <c r="M21">
-        <v>2.892290471792663</v>
+        <v>2.9475374507857901</v>
       </c>
       <c r="N21">
-        <v>2.862001271082785</v>
+        <v>2.9639012127436031</v>
       </c>
       <c r="O21">
-        <v>2.836168992466104</v>
+        <v>2.9477828042124119</v>
       </c>
       <c r="P21">
-        <v>2.825563827105859</v>
+        <v>2.9321773943201701</v>
       </c>
       <c r="Q21">
-        <v>2.782704388479197</v>
+        <v>2.8685900878111159</v>
       </c>
       <c r="R21">
-        <v>2.717544147784801</v>
+        <v>2.7805716574304968</v>
       </c>
       <c r="S21">
-        <v>2.644777707789272</v>
+        <v>2.6862074018584661</v>
       </c>
       <c r="T21">
-        <v>2.515847517177014</v>
+        <v>2.545077789937944</v>
       </c>
       <c r="U21">
-        <v>2.40579553017414</v>
+        <v>2.438932060980493</v>
       </c>
       <c r="V21">
-        <v>2.314058364017788</v>
+        <v>2.397448307555615</v>
       </c>
       <c r="W21">
-        <v>2.207493349536199</v>
+        <v>2.335326409406842</v>
       </c>
       <c r="X21">
-        <v>2.108658687361623</v>
+        <v>2.3344391965778009</v>
       </c>
       <c r="Y21">
-        <v>1.97453089849715</v>
+        <v>2.2405678688925779</v>
       </c>
       <c r="Z21">
-        <v>1.853303096449408</v>
+        <v>2.1250691553982199</v>
       </c>
       <c r="AA21">
-        <v>1.726543445412042</v>
+        <v>1.9676600747376849</v>
       </c>
       <c r="AB21">
-        <v>1.597739865333722</v>
+        <v>1.794721712389171</v>
       </c>
       <c r="AC21">
-        <v>1.497720264552575</v>
+        <v>1.656402644497728</v>
       </c>
       <c r="AD21">
-        <v>1.387009493041772</v>
+        <v>1.526692395357107</v>
       </c>
       <c r="AE21">
-        <v>1.295063990478784</v>
+        <v>1.427582836564627</v>
       </c>
       <c r="AF21">
-        <v>1.227075937526078</v>
+        <v>1.357771314701302</v>
       </c>
       <c r="AG21">
-        <v>1.166998850575423</v>
+        <v>1.303106783029345</v>
       </c>
       <c r="AH21">
-        <v>1.135863838506686</v>
+        <v>1.2918047226972109</v>
       </c>
       <c r="AI21">
-        <v>1.091959229465986</v>
+        <v>1.3910440226302481</v>
       </c>
       <c r="AJ21">
-        <v>1.034962107799708</v>
+        <v>1.3879417857775711</v>
       </c>
       <c r="AK21">
-        <v>1.006540440947026</v>
+        <v>1.327516434160759</v>
       </c>
       <c r="AL21">
-        <v>0.9583899003338321</v>
+        <v>1.1965330624649699</v>
       </c>
       <c r="AM21">
-        <v>0.9019750281761003</v>
+        <v>1.0353571648568101</v>
       </c>
       <c r="AN21">
-        <v>0.8507279941503073</v>
+        <v>0.89313654931279896</v>
       </c>
       <c r="AO21">
-        <v>0.8104412835035585</v>
+        <v>0.78811942926007916</v>
       </c>
       <c r="AP21">
-        <v>0.7728245845461853</v>
+        <v>0.71915415589639187</v>
       </c>
     </row>
-    <row r="22" spans="1:42">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.4875548940160001</v>
+        <v>0.43821573912399819</v>
       </c>
       <c r="D22">
-        <v>0.4953235346099318</v>
+        <v>0.4434740194859122</v>
       </c>
       <c r="E22">
-        <v>0.5042669884206106</v>
+        <v>0.4506175604103293</v>
       </c>
       <c r="F22">
-        <v>0.5139811273092615</v>
+        <v>0.45946169865589909</v>
       </c>
       <c r="G22">
-        <v>0.524021006964998</v>
+        <v>0.46964065541714078</v>
       </c>
       <c r="H22">
-        <v>0.5340263157303894</v>
+        <v>0.48045848753949078</v>
       </c>
       <c r="I22">
-        <v>0.5438125367718343</v>
+        <v>0.49158630685099741</v>
       </c>
       <c r="J22">
-        <v>0.5531512947335365</v>
+        <v>0.50294027272380648</v>
       </c>
       <c r="K22">
-        <v>0.5619955224142869</v>
+        <v>0.51415643301265423</v>
       </c>
       <c r="L22">
-        <v>0.5701803710741744</v>
+        <v>0.5245848586137497</v>
       </c>
       <c r="M22">
-        <v>0.5775821314832948</v>
+        <v>0.53407316274241989</v>
       </c>
       <c r="N22">
-        <v>0.583967332411639</v>
+        <v>0.54207738327408017</v>
       </c>
       <c r="O22">
-        <v>0.5892379932494712</v>
+        <v>0.54881275076858482</v>
       </c>
       <c r="P22">
-        <v>0.5927463092733819</v>
+        <v>0.55415486274119674</v>
       </c>
       <c r="Q22">
-        <v>0.5940313395992853</v>
+        <v>0.55854626868095458</v>
       </c>
       <c r="R22">
-        <v>0.5923920540437059</v>
+        <v>0.56213595593093113</v>
       </c>
       <c r="S22">
-        <v>0.5877389263841886</v>
+        <v>0.56475085608705744</v>
       </c>
       <c r="T22">
-        <v>0.5803984001081335</v>
+        <v>0.56690638302054053</v>
       </c>
       <c r="U22">
-        <v>0.5703478917616482</v>
+        <v>0.5682083534918797</v>
       </c>
       <c r="V22">
-        <v>0.5575914563172495</v>
+        <v>0.56832928081473921</v>
       </c>
       <c r="W22">
-        <v>0.5419758860684172</v>
+        <v>0.5664798733263785</v>
       </c>
       <c r="X22">
-        <v>0.5237464516218985</v>
+        <v>0.56180824046984335</v>
       </c>
       <c r="Y22">
-        <v>0.5033276208193848</v>
+        <v>0.5541424924548688</v>
       </c>
       <c r="Z22">
-        <v>0.4813371817191641</v>
+        <v>0.54328454638406209</v>
       </c>
       <c r="AA22">
-        <v>0.4583459190014997</v>
+        <v>0.52980771640863311</v>
       </c>
       <c r="AB22">
-        <v>0.4347729550364244</v>
+        <v>0.51400447480866807</v>
       </c>
       <c r="AC22">
-        <v>0.411061002672245</v>
+        <v>0.4959738957039615</v>
       </c>
       <c r="AD22">
-        <v>0.3876203271746761</v>
+        <v>0.47590605578056983</v>
       </c>
       <c r="AE22">
-        <v>0.3648322188924301</v>
+        <v>0.45411004229428642</v>
       </c>
       <c r="AF22">
-        <v>0.3430254912154377</v>
+        <v>0.43114023589102962</v>
       </c>
       <c r="AG22">
-        <v>0.3224281578895326</v>
+        <v>0.4077410773653104</v>
       </c>
       <c r="AH22">
-        <v>0.3032216876784832</v>
+        <v>0.3842994570778987</v>
       </c>
       <c r="AI22">
-        <v>0.2855555036093925</v>
+        <v>0.36082284441734169</v>
       </c>
       <c r="AJ22">
-        <v>0.2696267570658704</v>
+        <v>0.33802636458707419</v>
       </c>
       <c r="AK22">
-        <v>0.2552684292871011</v>
+        <v>0.31655694146412439</v>
       </c>
       <c r="AL22">
-        <v>0.2425866859762685</v>
+        <v>0.2971878449900886</v>
       </c>
       <c r="AM22">
-        <v>0.2315026252338689</v>
+        <v>0.28022712387053522</v>
       </c>
       <c r="AN22">
-        <v>0.2219090094593632</v>
+        <v>0.26562566331407672</v>
       </c>
       <c r="AO22">
-        <v>0.2135899861140665</v>
+        <v>0.25323787947883369</v>
       </c>
       <c r="AP22">
-        <v>0.206288423303591</v>
+        <v>0.24260568363508159</v>
       </c>
     </row>
-    <row r="23" spans="1:42">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -3189,264 +3253,264 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:42">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>3.927994250000002</v>
+        <v>4.1017838999999983</v>
       </c>
       <c r="D24">
-        <v>3.607326212705539</v>
+        <v>3.7121906559513458</v>
       </c>
       <c r="E24">
-        <v>3.349322502771293</v>
+        <v>3.3895241369917239</v>
       </c>
       <c r="F24">
-        <v>3.12083010105709</v>
+        <v>3.10752502202623</v>
       </c>
       <c r="G24">
-        <v>2.953744623413583</v>
+        <v>2.907243216399177</v>
       </c>
       <c r="H24">
-        <v>2.811629391100031</v>
+        <v>2.75063499661342</v>
       </c>
       <c r="I24">
-        <v>2.69165794658378</v>
+        <v>2.623254888700727</v>
       </c>
       <c r="J24">
-        <v>2.604771418806743</v>
+        <v>2.5301598574051658</v>
       </c>
       <c r="K24">
-        <v>2.485891962764385</v>
+        <v>2.4312897319969249</v>
       </c>
       <c r="L24">
-        <v>2.403729642876492</v>
+        <v>2.4398978829429421</v>
       </c>
       <c r="M24">
-        <v>2.314708340309368</v>
+        <v>2.4134642880433659</v>
       </c>
       <c r="N24">
-        <v>2.278033938671145</v>
+        <v>2.4218238294695191</v>
       </c>
       <c r="O24">
-        <v>2.246930999216634</v>
+        <v>2.3989700534438239</v>
       </c>
       <c r="P24">
-        <v>2.232817517832478</v>
+        <v>2.378022531578968</v>
       </c>
       <c r="Q24">
-        <v>2.188673048879912</v>
+        <v>2.3100438191301582</v>
       </c>
       <c r="R24">
-        <v>2.125152093741095</v>
+        <v>2.218435701499561</v>
       </c>
       <c r="S24">
-        <v>2.057038781405084</v>
+        <v>2.1214565457714021</v>
       </c>
       <c r="T24">
-        <v>1.935449117068881</v>
+        <v>1.9781714069173979</v>
       </c>
       <c r="U24">
-        <v>1.835447638412491</v>
+        <v>1.8707237074886089</v>
       </c>
       <c r="V24">
-        <v>1.756466907700537</v>
+        <v>1.829119026740871</v>
       </c>
       <c r="W24">
-        <v>1.665517463467784</v>
+        <v>1.7688465360804571</v>
       </c>
       <c r="X24">
-        <v>1.584912235739725</v>
+        <v>1.772630956107953</v>
       </c>
       <c r="Y24">
-        <v>1.471203277677765</v>
+        <v>1.686425376437704</v>
       </c>
       <c r="Z24">
-        <v>1.371965914730245</v>
+        <v>1.5817846090141521</v>
       </c>
       <c r="AA24">
-        <v>1.268197526410542</v>
+        <v>1.4378523583290459</v>
       </c>
       <c r="AB24">
-        <v>1.162966910297298</v>
+        <v>1.2807172375804969</v>
       </c>
       <c r="AC24">
-        <v>1.08665926188033</v>
+        <v>1.1604287487937619</v>
       </c>
       <c r="AD24">
-        <v>0.9993891658670954</v>
+        <v>1.0507863395765329</v>
       </c>
       <c r="AE24">
-        <v>0.9302317715863542</v>
+        <v>0.97347279427033584</v>
       </c>
       <c r="AF24">
-        <v>0.8840504463106404</v>
+        <v>0.92663107881026596</v>
       </c>
       <c r="AG24">
-        <v>0.8445706926858911</v>
+        <v>0.8953657056640294</v>
       </c>
       <c r="AH24">
-        <v>0.8326421508282029</v>
+        <v>0.90750526561930589</v>
       </c>
       <c r="AI24">
-        <v>0.806403725856594</v>
+        <v>1.0302211782129009</v>
       </c>
       <c r="AJ24">
-        <v>0.7653353507338375</v>
+        <v>1.049915421190492</v>
       </c>
       <c r="AK24">
-        <v>0.7512720116599242</v>
+        <v>1.010959492696629</v>
       </c>
       <c r="AL24">
-        <v>0.7158032143575637</v>
+        <v>0.8993452174748755</v>
       </c>
       <c r="AM24">
-        <v>0.6704724029422314</v>
+        <v>0.75513004098627001</v>
       </c>
       <c r="AN24">
-        <v>0.6288189846909441</v>
+        <v>0.62751088599871652</v>
       </c>
       <c r="AO24">
-        <v>0.5968512973894923</v>
+        <v>0.53488154978123992</v>
       </c>
       <c r="AP24">
-        <v>0.5665361612425939</v>
+        <v>0.47654847226130698</v>
       </c>
     </row>
-    <row r="25" spans="1:42">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
       <c r="C25">
-        <v>95.584450855984</v>
+        <v>95.460000360875995</v>
       </c>
       <c r="D25">
-        <v>91.48180110866851</v>
+        <v>91.30433568543873</v>
       </c>
       <c r="E25">
-        <v>87.62821161747659</v>
+        <v>87.464193988036669</v>
       </c>
       <c r="F25">
-        <v>83.99340038911026</v>
+        <v>83.897207267354531</v>
       </c>
       <c r="G25">
-        <v>80.51563475873168</v>
+        <v>80.520323395538199</v>
       </c>
       <c r="H25">
-        <v>77.16997905190125</v>
+        <v>77.289229911385277</v>
       </c>
       <c r="I25">
-        <v>73.93450856854568</v>
+        <v>74.174388715833544</v>
       </c>
       <c r="J25">
-        <v>70.77658585500537</v>
+        <v>71.141288585704558</v>
       </c>
       <c r="K25">
-        <v>67.7286983698267</v>
+        <v>68.195842420694973</v>
       </c>
       <c r="L25">
-        <v>64.75478835587602</v>
+        <v>65.231359679138279</v>
       </c>
       <c r="M25">
-        <v>61.86249788408337</v>
+        <v>62.283822228352477</v>
       </c>
       <c r="N25">
-        <v>59.00049661300058</v>
+        <v>59.31992101560887</v>
       </c>
       <c r="O25">
-        <v>56.16432762053451</v>
+        <v>56.372138211396447</v>
       </c>
       <c r="P25">
-        <v>53.33876379342862</v>
+        <v>53.439960817076283</v>
       </c>
       <c r="Q25">
-        <v>50.55605940494943</v>
+        <v>50.571370729265148</v>
       </c>
       <c r="R25">
-        <v>47.83851525716463</v>
+        <v>47.790799071834662</v>
       </c>
       <c r="S25">
-        <v>45.19373754937538</v>
+        <v>45.10459166997618</v>
       </c>
       <c r="T25">
-        <v>42.67789003219833</v>
+        <v>42.559513880038232</v>
       </c>
       <c r="U25">
-        <v>40.27209450202421</v>
+        <v>40.120581819057733</v>
       </c>
       <c r="V25">
-        <v>37.95803613800641</v>
+        <v>37.72313351150212</v>
       </c>
       <c r="W25">
-        <v>35.75054278847023</v>
+        <v>35.387807102095273</v>
       </c>
       <c r="X25">
-        <v>33.6418841011086</v>
+        <v>33.053367905517462</v>
       </c>
       <c r="Y25">
-        <v>31.66735320261144</v>
+        <v>30.812800036624878</v>
       </c>
       <c r="Z25">
-        <v>29.81405010616204</v>
+        <v>28.68773088122666</v>
       </c>
       <c r="AA25">
-        <v>28.08750666075</v>
+        <v>26.72007080648897</v>
       </c>
       <c r="AB25">
-        <v>26.48976679541626</v>
+        <v>24.92534909409979</v>
       </c>
       <c r="AC25">
-        <v>24.9920465308637</v>
+        <v>23.268946449602058</v>
       </c>
       <c r="AD25">
-        <v>23.60503703782193</v>
+        <v>21.742254054244949</v>
       </c>
       <c r="AE25">
-        <v>22.30997304734315</v>
+        <v>20.31467121768031</v>
       </c>
       <c r="AF25">
-        <v>21.08289710981706</v>
+        <v>18.956899902979</v>
       </c>
       <c r="AG25">
-        <v>19.91589825924164</v>
+        <v>17.653793119949661</v>
       </c>
       <c r="AH25">
-        <v>18.78003442073495</v>
+        <v>16.361988397252439</v>
       </c>
       <c r="AI25">
-        <v>17.68807519126896</v>
+        <v>14.97094437462219</v>
       </c>
       <c r="AJ25">
-        <v>16.65311308346925</v>
+        <v>13.583002588844611</v>
       </c>
       <c r="AK25">
-        <v>15.64657264252224</v>
+        <v>12.255486154683849</v>
       </c>
       <c r="AL25">
-        <v>14.68818274218839</v>
+        <v>11.05895309221888</v>
       </c>
       <c r="AM25">
-        <v>13.7862077140123</v>
+        <v>10.023595927362059</v>
       </c>
       <c r="AN25">
-        <v>12.93547971986199</v>
+        <v>9.130459378049256</v>
       </c>
       <c r="AO25">
-        <v>12.12503843635843</v>
+        <v>8.3423399487891707</v>
       </c>
       <c r="AP25">
-        <v>11.35221385181225</v>
+        <v>7.6231857928927749</v>
       </c>
     </row>
-    <row r="26" spans="1:42">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B26">
@@ -3456,249 +3520,249 @@
         <v>14199883.24327</v>
       </c>
       <c r="D26">
-        <v>13773569.7113036</v>
+        <v>14111151.03168831</v>
       </c>
       <c r="E26">
-        <v>13388008.60482744</v>
+        <v>14064028.516302601</v>
       </c>
       <c r="F26">
-        <v>13032743.41298762</v>
+        <v>14049664.32730386</v>
       </c>
       <c r="G26">
-        <v>12701532.37998237</v>
+        <v>14061382.740197361</v>
       </c>
       <c r="H26">
-        <v>12385240.14738346</v>
+        <v>14087265.980035471</v>
       </c>
       <c r="I26">
-        <v>12078002.41010359</v>
+        <v>14118751.800130431</v>
       </c>
       <c r="J26">
-        <v>11773566.7968324</v>
+        <v>14148641.192651501</v>
       </c>
       <c r="K26">
-        <v>11464111.98333823</v>
+        <v>14167132.11985884</v>
       </c>
       <c r="L26">
-        <v>11159050.01659572</v>
+        <v>14181308.33923416</v>
       </c>
       <c r="M26">
-        <v>10859947.6923961</v>
+        <v>14183371.292032329</v>
       </c>
       <c r="N26">
-        <v>10569282.41420611</v>
+        <v>14176848.666921159</v>
       </c>
       <c r="O26">
-        <v>10280725.38058105</v>
+        <v>14156121.64789591</v>
       </c>
       <c r="P26">
-        <v>9991528.41162893</v>
+        <v>14115940.952702969</v>
       </c>
       <c r="Q26">
-        <v>9691153.779319746</v>
+        <v>14037234.280246601</v>
       </c>
       <c r="R26">
-        <v>9380820.210467333</v>
+        <v>13923106.729342081</v>
       </c>
       <c r="S26">
-        <v>9055470.355980959</v>
+        <v>13769406.983990731</v>
       </c>
       <c r="T26">
-        <v>8717306.033265037</v>
+        <v>13585521.244889161</v>
       </c>
       <c r="U26">
-        <v>8382637.61378545</v>
+        <v>13396397.811397269</v>
       </c>
       <c r="V26">
-        <v>8054741.585114814</v>
+        <v>13202831.95521467</v>
       </c>
       <c r="W26">
-        <v>7732813.053735973</v>
+        <v>12995020.585179459</v>
       </c>
       <c r="X26">
-        <v>7422941.939477259</v>
+        <v>12774977.035298539</v>
       </c>
       <c r="Y26">
-        <v>7115815.024614751</v>
+        <v>12507421.335295171</v>
       </c>
       <c r="Z26">
-        <v>6820732.29135769</v>
+        <v>12221630.040321181</v>
       </c>
       <c r="AA26">
-        <v>6539738.280012023</v>
+        <v>11932549.464707229</v>
       </c>
       <c r="AB26">
-        <v>6276490.642826026</v>
+        <v>11661508.92328639</v>
       </c>
       <c r="AC26">
-        <v>6035619.496272657</v>
+        <v>11424906.771819251</v>
       </c>
       <c r="AD26">
-        <v>5815547.60256223</v>
+        <v>11220114.59842086</v>
       </c>
       <c r="AE26">
-        <v>5616294.127825579</v>
+        <v>11043512.97347321</v>
       </c>
       <c r="AF26">
-        <v>5432063.656487682</v>
+        <v>10881705.553554781</v>
       </c>
       <c r="AG26">
-        <v>5259880.444725553</v>
+        <v>10726278.26694216</v>
       </c>
       <c r="AH26">
-        <v>5095758.352302332</v>
+        <v>10561109.74978698</v>
       </c>
       <c r="AI26">
-        <v>4932147.484307316</v>
+        <v>10354968.81611553</v>
       </c>
       <c r="AJ26">
-        <v>4772890.083105937</v>
+        <v>10007692.53014956</v>
       </c>
       <c r="AK26">
-        <v>4619671.489675169</v>
+        <v>9576943.9886050262</v>
       </c>
       <c r="AL26">
-        <v>4463592.950929945</v>
+        <v>9100871.3294437733</v>
       </c>
       <c r="AM26">
-        <v>4310550.493863324</v>
+        <v>8644567.5236459747</v>
       </c>
       <c r="AN26">
-        <v>4162476.080827186</v>
+        <v>8251442.598735786</v>
       </c>
       <c r="AO26">
-        <v>4019222.705616066</v>
+        <v>7923994.6897185622</v>
       </c>
       <c r="AP26">
-        <v>3876428.950988912</v>
+        <v>7640264.3480006568</v>
       </c>
     </row>
-    <row r="27" spans="1:42">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>14199883.24327</v>
       </c>
       <c r="C27">
-        <v>13773569.7113036</v>
+        <v>14111151.03168831</v>
       </c>
       <c r="D27">
-        <v>13388008.60482744</v>
+        <v>14064028.516302601</v>
       </c>
       <c r="E27">
-        <v>13032743.41298762</v>
+        <v>14049664.32730386</v>
       </c>
       <c r="F27">
-        <v>12701532.37998237</v>
+        <v>14061382.740197361</v>
       </c>
       <c r="G27">
-        <v>12385240.14738346</v>
+        <v>14087265.980035471</v>
       </c>
       <c r="H27">
-        <v>12078002.41010359</v>
+        <v>14118751.800130431</v>
       </c>
       <c r="I27">
-        <v>11773566.7968324</v>
+        <v>14148641.192651501</v>
       </c>
       <c r="J27">
-        <v>11464111.98333823</v>
+        <v>14167132.11985884</v>
       </c>
       <c r="K27">
-        <v>11159050.01659572</v>
+        <v>14181308.33923416</v>
       </c>
       <c r="L27">
-        <v>10859947.6923961</v>
+        <v>14183371.292032329</v>
       </c>
       <c r="M27">
-        <v>10569282.41420611</v>
+        <v>14176848.666921159</v>
       </c>
       <c r="N27">
-        <v>10280725.38058105</v>
+        <v>14156121.64789591</v>
       </c>
       <c r="O27">
-        <v>9991528.41162893</v>
+        <v>14115940.952702969</v>
       </c>
       <c r="P27">
-        <v>9691153.779319746</v>
+        <v>14037234.280246601</v>
       </c>
       <c r="Q27">
-        <v>9380820.210467333</v>
+        <v>13923106.729342081</v>
       </c>
       <c r="R27">
-        <v>9055470.355980959</v>
+        <v>13769406.983990731</v>
       </c>
       <c r="S27">
-        <v>8717306.033265037</v>
+        <v>13585521.244889161</v>
       </c>
       <c r="T27">
-        <v>8382637.61378545</v>
+        <v>13396397.811397269</v>
       </c>
       <c r="U27">
-        <v>8054741.585114814</v>
+        <v>13202831.95521467</v>
       </c>
       <c r="V27">
-        <v>7732813.053735973</v>
+        <v>12995020.585179459</v>
       </c>
       <c r="W27">
-        <v>7422941.939477259</v>
+        <v>12774977.035298539</v>
       </c>
       <c r="X27">
-        <v>7115815.024614751</v>
+        <v>12507421.335295171</v>
       </c>
       <c r="Y27">
-        <v>6820732.29135769</v>
+        <v>12221630.040321181</v>
       </c>
       <c r="Z27">
-        <v>6539738.280012023</v>
+        <v>11932549.464707229</v>
       </c>
       <c r="AA27">
-        <v>6276490.642826026</v>
+        <v>11661508.92328639</v>
       </c>
       <c r="AB27">
-        <v>6035619.496272657</v>
+        <v>11424906.771819251</v>
       </c>
       <c r="AC27">
-        <v>5815547.60256223</v>
+        <v>11220114.59842086</v>
       </c>
       <c r="AD27">
-        <v>5616294.127825579</v>
+        <v>11043512.97347321</v>
       </c>
       <c r="AE27">
-        <v>5432063.656487682</v>
+        <v>10881705.553554781</v>
       </c>
       <c r="AF27">
-        <v>5259880.444725553</v>
+        <v>10726278.26694216</v>
       </c>
       <c r="AG27">
-        <v>5095758.352302332</v>
+        <v>10561109.74978698</v>
       </c>
       <c r="AH27">
-        <v>4932147.484307316</v>
+        <v>10354968.81611553</v>
       </c>
       <c r="AI27">
-        <v>4772890.083105937</v>
+        <v>10007692.53014956</v>
       </c>
       <c r="AJ27">
-        <v>4619671.489675169</v>
+        <v>9576943.9886050262</v>
       </c>
       <c r="AK27">
-        <v>4463592.950929945</v>
+        <v>9100871.3294437733</v>
       </c>
       <c r="AL27">
-        <v>4310550.493863324</v>
+        <v>8644567.5236459747</v>
       </c>
       <c r="AM27">
-        <v>4162476.080827186</v>
+        <v>8251442.598735786</v>
       </c>
       <c r="AN27">
-        <v>4019222.705616066</v>
+        <v>7923994.6897185622</v>
       </c>
       <c r="AO27">
-        <v>3876428.950988912</v>
+        <v>7640264.3480006568</v>
       </c>
       <c r="AP27">
-        <v>3734815.053416233</v>
+        <v>7369932.8182373242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- implementation du resultat technique apres PB!!!
</commit_message>
<xml_diff>
--- a/tests/output_test_data/mp_global_projection_reporting.xlsx
+++ b/tests/output_test_data/mp_global_projection_reporting.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef77bd1ebbbb3aed/Modele_ALM/tests/output_test_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_FFC65FC05B79ECDE962EABFC8A2F55C961B401BC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4628842-15A6-964A-9B3F-4200153F728A}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="1520" windowWidth="23860" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" calcCompleted="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>annee</t>
   </si>
@@ -99,12 +93,18 @@
   <si>
     <t>X/ Provision mathematiques de cloture</t>
   </si>
+  <si>
+    <t>XX/Resultat technique</t>
+  </si>
+  <si>
+    <t>XXX/Resultat technique après PB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,19 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -176,19 +167,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -230,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,27 +245,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,24 +279,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,66 +454,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AP29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="37.6640625" style="4" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:42">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:42">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -693,8 +635,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:42">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -821,8 +763,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:42">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -949,8 +891,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:42">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -1077,520 +1019,520 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:42">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>43518.266528369917</v>
+        <v>43518.26652836992</v>
       </c>
       <c r="D7">
-        <v>43418.11064879295</v>
+        <v>43412.29593179695</v>
       </c>
       <c r="E7">
-        <v>43429.354720710689</v>
+        <v>43417.98732305297</v>
       </c>
       <c r="F7">
-        <v>43524.93153912251</v>
+        <v>43508.2507142561</v>
       </c>
       <c r="G7">
-        <v>43666.16642959146</v>
+        <v>43644.39351534169</v>
       </c>
       <c r="H7">
-        <v>43832.473282778687</v>
+        <v>43805.82308556153</v>
       </c>
       <c r="I7">
-        <v>44009.973621243313</v>
+        <v>43978.64299947037</v>
       </c>
       <c r="J7">
-        <v>44150.992552086253</v>
+        <v>44115.15818105368</v>
       </c>
       <c r="K7">
-        <v>44276.491336901257</v>
+        <v>44239.36017073406</v>
       </c>
       <c r="L7">
-        <v>44353.918951318206</v>
+        <v>44315.53066096151</v>
       </c>
       <c r="M7">
-        <v>44392.622001896038</v>
+        <v>44353.06001792177</v>
       </c>
       <c r="N7">
-        <v>44368.166259867037</v>
+        <v>44327.61853414684</v>
       </c>
       <c r="O7">
-        <v>44273.204296472257</v>
+        <v>44231.82413890408</v>
       </c>
       <c r="P7">
-        <v>44086.020948839949</v>
+        <v>44044.00800991992</v>
       </c>
       <c r="Q7">
-        <v>43795.060448787794</v>
+        <v>43752.69632696603</v>
       </c>
       <c r="R7">
-        <v>43399.583817342187</v>
+        <v>43356.999969367</v>
       </c>
       <c r="S7">
-        <v>42936.552075322099</v>
+        <v>42893.7805619814</v>
       </c>
       <c r="T7">
-        <v>42465.015671323978</v>
+        <v>42421.99657702713</v>
       </c>
       <c r="U7">
-        <v>41965.91719964247</v>
+        <v>41922.62268615082</v>
       </c>
       <c r="V7">
-        <v>41401.314731858532</v>
+        <v>41357.822725473</v>
       </c>
       <c r="W7">
-        <v>40779.52969886014</v>
+        <v>40736.0409413588</v>
       </c>
       <c r="X7">
-        <v>40025.36336445839</v>
+        <v>39982.20485759115</v>
       </c>
       <c r="Y7">
-        <v>39235.834054352817</v>
+        <v>39193.17835641678</v>
       </c>
       <c r="Z7">
-        <v>38463.688802030963</v>
+        <v>38421.57662442009</v>
       </c>
       <c r="AA7">
-        <v>37768.983599308507</v>
+        <v>37727.33600663445</v>
       </c>
       <c r="AB7">
-        <v>37186.46938146621</v>
+        <v>37145.12941578074</v>
       </c>
       <c r="AC7">
-        <v>36691.065552478853</v>
+        <v>36649.89822044031</v>
       </c>
       <c r="AD7">
-        <v>36272.666129374178</v>
+        <v>36231.59683428128</v>
       </c>
       <c r="AE7">
-        <v>35897.548614317537</v>
+        <v>35856.64638718151</v>
       </c>
       <c r="AF7">
-        <v>35540.884833702134</v>
+        <v>35500.26466265512</v>
       </c>
       <c r="AG7">
-        <v>35140.434881312452</v>
+        <v>35100.32711190868</v>
       </c>
       <c r="AH7">
-        <v>34590.101311198523</v>
+        <v>34550.75180975247</v>
       </c>
       <c r="AI7">
-        <v>33490.530299685961</v>
+        <v>33452.47724450655</v>
       </c>
       <c r="AJ7">
-        <v>32056.16063937057</v>
+        <v>32019.69699269229</v>
       </c>
       <c r="AK7">
-        <v>30430.900550146729</v>
+        <v>30396.15676465204</v>
       </c>
       <c r="AL7">
-        <v>28864.853107317718</v>
+        <v>28831.74474631324</v>
       </c>
       <c r="AM7">
-        <v>27527.7462852235</v>
+        <v>27496.0664823324</v>
       </c>
       <c r="AN7">
-        <v>26433.02651942318</v>
+        <v>26402.57296275526</v>
       </c>
       <c r="AO7">
-        <v>25497.798078377989</v>
+        <v>25468.44358429882</v>
       </c>
       <c r="AP7">
-        <v>24611.225583912928</v>
+        <v>24582.93610131355</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:42">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>18236.888884505959</v>
+        <v>18236.88888450596</v>
       </c>
       <c r="D8">
-        <v>16994.14413989905</v>
+        <v>16992.06024531795</v>
       </c>
       <c r="E8">
-        <v>16009.235326458889</v>
+        <v>16005.26787842381</v>
       </c>
       <c r="F8">
-        <v>15270.85137769514</v>
+        <v>15265.19178190262</v>
       </c>
       <c r="G8">
-        <v>14863.548755779209</v>
+        <v>14856.36471430728</v>
       </c>
       <c r="H8">
-        <v>14726.12125210565</v>
+        <v>14717.31340553223</v>
       </c>
       <c r="I8">
-        <v>14787.972862989751</v>
+        <v>14777.75746855638</v>
       </c>
       <c r="J8">
-        <v>15097.06756309861</v>
+        <v>15085.63999180945</v>
       </c>
       <c r="K8">
-        <v>15162.878327500401</v>
+        <v>15151.39687613861</v>
       </c>
       <c r="L8">
-        <v>15538.41944917006</v>
+        <v>15526.54140814325</v>
       </c>
       <c r="M8">
-        <v>15711.92895460111</v>
+        <v>15699.40522268774</v>
       </c>
       <c r="N8">
-        <v>16188.19762194252</v>
+        <v>16173.84159675986</v>
       </c>
       <c r="O8">
-        <v>16829.63060536531</v>
+        <v>16813.90051302091</v>
       </c>
       <c r="P8">
-        <v>18025.966742868441</v>
+        <v>18007.91241095572</v>
       </c>
       <c r="Q8">
-        <v>18700.592634724049</v>
+        <v>18681.04244700287</v>
       </c>
       <c r="R8">
-        <v>19259.569973970301</v>
+        <v>19239.62155495919</v>
       </c>
       <c r="S8">
-        <v>19250.73810375739</v>
+        <v>19231.39712590184</v>
       </c>
       <c r="T8">
-        <v>18636.276017775181</v>
+        <v>18618.05757496181</v>
       </c>
       <c r="U8">
-        <v>18109.843180915821</v>
+        <v>18092.17845294107</v>
       </c>
       <c r="V8">
-        <v>18074.362159489028</v>
+        <v>18055.86030480351</v>
       </c>
       <c r="W8">
-        <v>18023.53590584937</v>
+        <v>18003.65585491746</v>
       </c>
       <c r="X8">
-        <v>19034.031066505639</v>
+        <v>19010.7647422623</v>
       </c>
       <c r="Y8">
-        <v>19110.46764097819</v>
+        <v>19085.85066011832</v>
       </c>
       <c r="Z8">
-        <v>18758.285343178432</v>
+        <v>18733.67984124411</v>
       </c>
       <c r="AA8">
-        <v>17766.954299609049</v>
+        <v>17743.76302493224</v>
       </c>
       <c r="AB8">
-        <v>16436.306062423519</v>
+        <v>16415.33867587501</v>
       </c>
       <c r="AC8">
-        <v>15413.583530954509</v>
+        <v>15394.50300966386</v>
       </c>
       <c r="AD8">
-        <v>14572.188833600891</v>
+        <v>14554.08961387167</v>
       </c>
       <c r="AE8">
-        <v>14252.835137839829</v>
+        <v>14233.51139990564</v>
       </c>
       <c r="AF8">
-        <v>14060.72493416512</v>
+        <v>14040.45394202893</v>
       </c>
       <c r="AG8">
-        <v>14209.58798648576</v>
+        <v>14188.40069992645</v>
       </c>
       <c r="AH8">
-        <v>15243.298575986981</v>
+        <v>15221.67736261799</v>
       </c>
       <c r="AI8">
-        <v>19102.38802984446</v>
+        <v>19079.58088797403</v>
       </c>
       <c r="AJ8">
-        <v>21160.632329690819</v>
+        <v>21138.02449365593</v>
       </c>
       <c r="AK8">
-        <v>22023.65621389763</v>
+        <v>22001.88395759688</v>
       </c>
       <c r="AL8">
-        <v>20927.805100093239</v>
+        <v>20907.61110576967</v>
       </c>
       <c r="AM8">
-        <v>18544.884646917861</v>
+        <v>18526.60828938101</v>
       </c>
       <c r="AN8">
-        <v>16115.450071526609</v>
+        <v>16098.9613104157</v>
       </c>
       <c r="AO8">
-        <v>14365.91208553238</v>
+        <v>14350.94189453342</v>
       </c>
       <c r="AP8">
-        <v>13517.42367905319</v>
+        <v>13503.42940180152</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:42">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>692067.61839274841</v>
+        <v>692067.6183927484</v>
       </c>
       <c r="D9">
-        <v>652965.9982048251</v>
+        <v>652885.1219209414</v>
       </c>
       <c r="E9">
-        <v>624475.39044221235</v>
+        <v>624319.7913651573</v>
       </c>
       <c r="F9">
-        <v>603980.58127964265</v>
+        <v>603757.0828925594</v>
       </c>
       <c r="G9">
-        <v>596065.32379051135</v>
+        <v>595780.2214593596</v>
       </c>
       <c r="H9">
-        <v>596999.76485372894</v>
+        <v>596651.7595729996</v>
       </c>
       <c r="I9">
-        <v>604863.63765360159</v>
+        <v>604460.9611748881</v>
       </c>
       <c r="J9">
-        <v>621773.80204239243</v>
+        <v>621321.6367739176</v>
       </c>
       <c r="K9">
-        <v>631279.05442036584</v>
+        <v>630819.4190569355</v>
       </c>
       <c r="L9">
-        <v>648017.79567084811</v>
+        <v>647539.9685154526</v>
       </c>
       <c r="M9">
-        <v>661037.64804282307</v>
+        <v>660527.0379810743</v>
       </c>
       <c r="N9">
-        <v>679504.01688370423</v>
+        <v>678935.2393232954</v>
       </c>
       <c r="O9">
-        <v>702448.32011735975</v>
+        <v>701834.8238566491</v>
       </c>
       <c r="P9">
-        <v>742739.96515234304</v>
+        <v>742067.1494573568</v>
       </c>
       <c r="Q9">
-        <v>778052.04695131746</v>
+        <v>777313.7629572867</v>
       </c>
       <c r="R9">
-        <v>814758.22578941646</v>
+        <v>813994.9062365444</v>
       </c>
       <c r="S9">
-        <v>839754.09391442104</v>
+        <v>838994.0145226673</v>
       </c>
       <c r="T9">
-        <v>838936.78087834269</v>
+        <v>838200.7962664922</v>
       </c>
       <c r="U9">
-        <v>836983.37654471945</v>
+        <v>836258.7593762274</v>
       </c>
       <c r="V9">
-        <v>844487.37590033188</v>
+        <v>843739.704330378</v>
       </c>
       <c r="W9">
-        <v>849904.66100712225</v>
+        <v>849106.3644729696</v>
       </c>
       <c r="X9">
-        <v>888585.14652144071</v>
+        <v>887696.510818648</v>
       </c>
       <c r="Y9">
-        <v>897050.01761251083</v>
+        <v>896124.660864271</v>
       </c>
       <c r="Z9">
-        <v>890063.1378152417</v>
+        <v>889141.360556297</v>
       </c>
       <c r="AA9">
-        <v>862349.63051614189</v>
+        <v>861463.0702248877</v>
       </c>
       <c r="AB9">
-        <v>819769.75508785388</v>
+        <v>818940.6621310525</v>
       </c>
       <c r="AC9">
-        <v>781431.88989497756</v>
+        <v>780650.7993370276</v>
       </c>
       <c r="AD9">
-        <v>748271.93366428697</v>
+        <v>747518.2124033918</v>
       </c>
       <c r="AE9">
-        <v>729571.23230321577</v>
+        <v>728796.0781191612</v>
       </c>
       <c r="AF9">
-        <v>719864.55760604877</v>
+        <v>719062.049758772</v>
       </c>
       <c r="AG9">
-        <v>725858.87282712781</v>
+        <v>725009.2414571035</v>
       </c>
       <c r="AH9">
-        <v>760855.47738972504</v>
+        <v>759961.9676658513</v>
       </c>
       <c r="AI9">
-        <v>887475.92735273985</v>
+        <v>886477.0063798418</v>
       </c>
       <c r="AJ9">
-        <v>951045.21447156824</v>
+        <v>950012.1725814287</v>
       </c>
       <c r="AK9">
-        <v>973166.57693948376</v>
+        <v>972142.7039905339</v>
       </c>
       <c r="AL9">
-        <v>930765.25278711761</v>
+        <v>929801.8816209611</v>
       </c>
       <c r="AM9">
-        <v>848249.964277972</v>
+        <v>847372.1154512733</v>
       </c>
       <c r="AN9">
-        <v>766836.75929602585</v>
+        <v>766037.600282595</v>
       </c>
       <c r="AO9">
-        <v>709743.68372374203</v>
+        <v>709001.27597745</v>
       </c>
       <c r="AP9">
-        <v>683540.65340311592</v>
+        <v>682828.942528024</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:42">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>60078.447224256808</v>
+        <v>60078.44722425681</v>
       </c>
       <c r="D10">
-        <v>63271.306967338809</v>
+        <v>63264.48547014929</v>
       </c>
       <c r="E10">
-        <v>66988.616654839934</v>
+        <v>66974.73898790366</v>
       </c>
       <c r="F10">
-        <v>71263.104066607862</v>
+        <v>71241.83712215966</v>
       </c>
       <c r="G10">
-        <v>76081.635828863029</v>
+        <v>76052.52698264421</v>
       </c>
       <c r="H10">
-        <v>81380.876380341608</v>
+        <v>81343.40340606689</v>
       </c>
       <c r="I10">
-        <v>87117.649889090113</v>
+        <v>87071.20475958619</v>
       </c>
       <c r="J10">
-        <v>93283.01354195163</v>
+        <v>93226.90633523457</v>
       </c>
       <c r="K10">
-        <v>99883.216452721143</v>
+        <v>99821.74596841617</v>
       </c>
       <c r="L10">
-        <v>106857.7911642737</v>
+        <v>106790.6351526799</v>
       </c>
       <c r="M10">
-        <v>114199.8131248892</v>
+        <v>114126.7411066546</v>
       </c>
       <c r="N10">
-        <v>121790.3767715532</v>
+        <v>121711.3108959111</v>
       </c>
       <c r="O10">
-        <v>129592.59724021101</v>
+        <v>129507.4689466079</v>
       </c>
       <c r="P10">
-        <v>137512.99345342189</v>
+        <v>137421.8177121507</v>
       </c>
       <c r="Q10">
-        <v>145585.05046305171</v>
+        <v>145487.9481971177</v>
       </c>
       <c r="R10">
-        <v>153784.59802463351</v>
+        <v>153681.563677494</v>
       </c>
       <c r="S10">
-        <v>162068.23167367341</v>
+        <v>161959.1972307824</v>
       </c>
       <c r="T10">
-        <v>170638.0256319477</v>
+        <v>170522.6488444966</v>
       </c>
       <c r="U10">
-        <v>179492.128764503</v>
+        <v>179370.1174784617</v>
       </c>
       <c r="V10">
-        <v>188660.45333578839</v>
+        <v>188531.6275397149</v>
       </c>
       <c r="W10">
-        <v>197881.85065221961</v>
+        <v>197746.2937335173</v>
       </c>
       <c r="X10">
-        <v>206693.9728184772</v>
+        <v>206552.0506655953</v>
       </c>
       <c r="Y10">
-        <v>214808.27879314471</v>
+        <v>214660.2820488999</v>
       </c>
       <c r="Z10">
-        <v>221974.384325472</v>
+        <v>221820.5803833973</v>
       </c>
       <c r="AA10">
-        <v>228246.5804009219</v>
+        <v>228087.0815569913</v>
       </c>
       <c r="AB10">
-        <v>233616.1753916525</v>
+        <v>233451.1213556448</v>
       </c>
       <c r="AC10">
-        <v>237949.4434944794</v>
+        <v>237779.1650154293</v>
       </c>
       <c r="AD10">
-        <v>241027.0402085621</v>
+        <v>240852.0634961792</v>
       </c>
       <c r="AE10">
-        <v>242659.11365682489</v>
+        <v>242480.2650681304</v>
       </c>
       <c r="AF10">
-        <v>242904.542682536</v>
+        <v>242722.7200406561</v>
       </c>
       <c r="AG10">
-        <v>241989.6530546275</v>
+        <v>241805.6233513296</v>
       </c>
       <c r="AH10">
-        <v>240059.99822815479</v>
+        <v>239874.4335696287</v>
       </c>
       <c r="AI10">
-        <v>237007.52599080201</v>
+        <v>236821.2612895963</v>
       </c>
       <c r="AJ10">
-        <v>233203.59523136151</v>
+        <v>233017.1188554809</v>
       </c>
       <c r="AK10">
-        <v>229158.75958892429</v>
+        <v>228972.2246290971</v>
       </c>
       <c r="AL10">
-        <v>225645.42531574689</v>
+        <v>225458.4725790109</v>
       </c>
       <c r="AM10">
-        <v>223166.9897175502</v>
+        <v>222979.0095404983</v>
       </c>
       <c r="AN10">
-        <v>221982.40883578151</v>
+        <v>221792.6356597332</v>
       </c>
       <c r="AO10">
-        <v>222193.70535131681</v>
+        <v>222001.2341870525</v>
       </c>
       <c r="AP10">
-        <v>223612.96669978549</v>
+        <v>223417.039134891</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:42">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1717,264 +1659,264 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:42">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>33854.174498439228</v>
+        <v>33854.17449843923</v>
       </c>
       <c r="D12">
-        <v>33729.787051337044</v>
+        <v>33725.04429598154</v>
       </c>
       <c r="E12">
-        <v>33683.090541003483</v>
+        <v>33673.85327256461</v>
       </c>
       <c r="F12">
-        <v>33698.4555038201</v>
+        <v>33684.95647594413</v>
       </c>
       <c r="G12">
-        <v>33747.662697761531</v>
+        <v>33730.11647982812</v>
       </c>
       <c r="H12">
-        <v>33810.191015493088</v>
+        <v>33788.80943732307</v>
       </c>
       <c r="I12">
-        <v>33869.393890919368</v>
+        <v>33844.36710991216</v>
       </c>
       <c r="J12">
-        <v>33901.923284734599</v>
+        <v>33873.42060055761</v>
       </c>
       <c r="K12">
-        <v>33924.443773028746</v>
+        <v>33895.1415035551</v>
       </c>
       <c r="L12">
-        <v>33918.021412439368</v>
+        <v>33887.95330358425</v>
       </c>
       <c r="M12">
-        <v>33890.560511251897</v>
+        <v>33859.79621698378</v>
       </c>
       <c r="N12">
-        <v>33827.931453727957</v>
+        <v>33796.60687977188</v>
       </c>
       <c r="O12">
-        <v>33718.479518241977</v>
+        <v>33686.70507967934</v>
       </c>
       <c r="P12">
-        <v>33516.794455014111</v>
+        <v>33484.72248295412</v>
       </c>
       <c r="Q12">
-        <v>33231.033166153589</v>
+        <v>33198.84325246241</v>
       </c>
       <c r="R12">
-        <v>32853.003768302413</v>
+        <v>32820.78247587114</v>
       </c>
       <c r="S12">
-        <v>32405.145087910561</v>
+        <v>32372.90764889626</v>
       </c>
       <c r="T12">
-        <v>31946.32697747073</v>
+        <v>31914.02928415975</v>
       </c>
       <c r="U12">
-        <v>31477.229160031438</v>
+        <v>31444.85047434807</v>
       </c>
       <c r="V12">
-        <v>30973.294684998331</v>
+        <v>30940.89933027359</v>
       </c>
       <c r="W12">
-        <v>30438.887028000849</v>
+        <v>30406.61216048189</v>
       </c>
       <c r="X12">
-        <v>29790.455861596751</v>
+        <v>29758.54730241984</v>
       </c>
       <c r="Y12">
-        <v>29098.674981660792</v>
+        <v>29067.26224039578</v>
       </c>
       <c r="Z12">
-        <v>28399.917048887051</v>
+        <v>28369.03556589234</v>
       </c>
       <c r="AA12">
-        <v>27744.861739827302</v>
+        <v>27714.4675896497</v>
       </c>
       <c r="AB12">
-        <v>27172.278617038941</v>
+        <v>27142.2679913697</v>
       </c>
       <c r="AC12">
-        <v>26675.37564392047</v>
+        <v>26645.65996629279</v>
       </c>
       <c r="AD12">
-        <v>26245.219711169349</v>
+        <v>26215.75438391966</v>
       </c>
       <c r="AE12">
-        <v>25849.478048045112</v>
+        <v>25820.33576676426</v>
       </c>
       <c r="AF12">
-        <v>25468.273172803849</v>
+        <v>25439.54345946969</v>
       </c>
       <c r="AG12">
-        <v>25063.70775467428</v>
+        <v>25035.53364994671</v>
       </c>
       <c r="AH12">
-        <v>24562.04078295052</v>
+        <v>24534.56945726194</v>
       </c>
       <c r="AI12">
-        <v>23728.05235278896</v>
+        <v>23701.5992962362</v>
       </c>
       <c r="AJ12">
-        <v>22698.36419969421</v>
+        <v>22673.08922389366</v>
       </c>
       <c r="AK12">
-        <v>21563.351908936202</v>
+        <v>21539.31627681807</v>
       </c>
       <c r="AL12">
-        <v>20476.456332472819</v>
+        <v>20453.59294802108</v>
       </c>
       <c r="AM12">
-        <v>19539.643005934839</v>
+        <v>19517.81313896473</v>
       </c>
       <c r="AN12">
-        <v>18758.410625162309</v>
+        <v>18737.480684761</v>
       </c>
       <c r="AO12">
-        <v>18080.829588959448</v>
+        <v>18060.71114133664</v>
       </c>
       <c r="AP12">
-        <v>17435.3977308209</v>
+        <v>17416.06172902874</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:42">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>598134.99667005229</v>
+        <v>598134.9966700523</v>
       </c>
       <c r="D13">
-        <v>555964.90418614924</v>
+        <v>555895.5921548107</v>
       </c>
       <c r="E13">
-        <v>523803.68324636889</v>
+        <v>523671.1991046891</v>
       </c>
       <c r="F13">
-        <v>499019.02170921472</v>
+        <v>498830.2892944556</v>
       </c>
       <c r="G13">
-        <v>486236.02526388672</v>
+        <v>485997.5779968873</v>
       </c>
       <c r="H13">
-        <v>481808.69745789422</v>
+        <v>481519.5467296095</v>
       </c>
       <c r="I13">
-        <v>483876.59387359209</v>
+        <v>483545.3893053897</v>
       </c>
       <c r="J13">
-        <v>494588.86521570617</v>
+        <v>494221.3098381254</v>
       </c>
       <c r="K13">
-        <v>497471.39419461589</v>
+        <v>497102.5315849642</v>
       </c>
       <c r="L13">
-        <v>507241.98309413512</v>
+        <v>506861.3800591885</v>
       </c>
       <c r="M13">
-        <v>512947.27440668189</v>
+        <v>512540.500657436</v>
       </c>
       <c r="N13">
-        <v>523885.70865842298</v>
+        <v>523427.3215476124</v>
       </c>
       <c r="O13">
-        <v>539137.24335890682</v>
+        <v>538640.6498303619</v>
       </c>
       <c r="P13">
-        <v>571710.177243907</v>
+        <v>571160.609262252</v>
       </c>
       <c r="Q13">
-        <v>599235.96332211222</v>
+        <v>598626.9715077066</v>
       </c>
       <c r="R13">
-        <v>628120.62399648048</v>
+        <v>627492.5600831793</v>
       </c>
       <c r="S13">
-        <v>645280.71715283708</v>
+        <v>644661.9096429886</v>
       </c>
       <c r="T13">
-        <v>636352.42826892424</v>
+        <v>635764.1181378358</v>
       </c>
       <c r="U13">
-        <v>626014.01862018497</v>
+        <v>625443.7914234176</v>
       </c>
       <c r="V13">
-        <v>624853.62787954521</v>
+        <v>624267.1774603894</v>
       </c>
       <c r="W13">
-        <v>621583.92332690186</v>
+        <v>620953.4585789704</v>
       </c>
       <c r="X13">
-        <v>652100.71784136677</v>
+        <v>651385.9128506329</v>
       </c>
       <c r="Y13">
-        <v>653143.06383770541</v>
+        <v>652397.1165749753</v>
       </c>
       <c r="Z13">
-        <v>639688.83644088265</v>
+        <v>638951.7446070072</v>
       </c>
       <c r="AA13">
-        <v>606358.1883753927</v>
+        <v>605661.5210782468</v>
       </c>
       <c r="AB13">
-        <v>558981.3010791624</v>
+        <v>558347.272784038</v>
       </c>
       <c r="AC13">
-        <v>516807.07075657771</v>
+        <v>516225.9743553055</v>
       </c>
       <c r="AD13">
-        <v>480999.6737445555</v>
+        <v>480450.394523293</v>
       </c>
       <c r="AE13">
-        <v>461062.64059834578</v>
+        <v>460495.4772842665</v>
       </c>
       <c r="AF13">
-        <v>451491.74175070901</v>
+        <v>450899.7862586462</v>
       </c>
       <c r="AG13">
-        <v>458805.51201782603</v>
+        <v>458168.0844558271</v>
       </c>
       <c r="AH13">
-        <v>496233.43837861973</v>
+        <v>495552.9646389607</v>
       </c>
       <c r="AI13">
-        <v>626740.34900914889</v>
+        <v>625954.1457940093</v>
       </c>
       <c r="AJ13">
-        <v>695143.25504051254</v>
+        <v>694321.9645020542</v>
       </c>
       <c r="AK13">
-        <v>722444.46544162324</v>
+        <v>721631.1630846189</v>
       </c>
       <c r="AL13">
-        <v>684643.37113889796</v>
+        <v>683889.8160939292</v>
       </c>
       <c r="AM13">
-        <v>605543.33155448688</v>
+        <v>604875.2927718103</v>
       </c>
       <c r="AN13">
-        <v>526095.93983508216</v>
+        <v>525507.4839381009</v>
       </c>
       <c r="AO13">
-        <v>469469.14878346567</v>
+        <v>468939.3306490608</v>
       </c>
       <c r="AP13">
-        <v>442492.28897250962</v>
+        <v>441995.8416641043</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:42">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -2101,8 +2043,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:42">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -2229,8 +2171,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:42">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -2357,8 +2299,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:42">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
@@ -2485,8 +2427,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:42">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -2613,8 +2555,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:42">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
@@ -2741,149 +2683,149 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:42">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>31749.302369869401</v>
+        <v>31650.64058633286</v>
       </c>
       <c r="D20">
-        <v>31881.4818103709</v>
+        <v>31783.92489588417</v>
       </c>
       <c r="E20">
-        <v>32106.270836790631</v>
+        <v>32009.85584426253</v>
       </c>
       <c r="F20">
-        <v>32400.53035843961</v>
+        <v>32305.21384258277</v>
       </c>
       <c r="G20">
-        <v>32729.609746647471</v>
+        <v>32635.2762954466</v>
       </c>
       <c r="H20">
-        <v>33073.813094092278</v>
+        <v>32980.44592304926</v>
       </c>
       <c r="I20">
-        <v>33403.8165239031</v>
+        <v>33311.26208112891</v>
       </c>
       <c r="J20">
-        <v>33694.028813712277</v>
+        <v>33654.40597407973</v>
       </c>
       <c r="K20">
-        <v>33967.326803822289</v>
+        <v>33927.43730450812</v>
       </c>
       <c r="L20">
-        <v>34210.87975511339</v>
+        <v>34170.71111697288</v>
       </c>
       <c r="M20">
-        <v>34444.375937594377</v>
+        <v>34403.98213651299</v>
       </c>
       <c r="N20">
-        <v>34668.822335900382</v>
+        <v>34628.37028467986</v>
       </c>
       <c r="O20">
-        <v>34852.67680313965</v>
+        <v>34812.2753043321</v>
       </c>
       <c r="P20">
-        <v>34945.7508856985</v>
+        <v>34905.64104426717</v>
       </c>
       <c r="Q20">
-        <v>34940.179106597207</v>
+        <v>34900.53042977249</v>
       </c>
       <c r="R20">
-        <v>34789.478611010811</v>
+        <v>34750.28398801642</v>
       </c>
       <c r="S20">
-        <v>34516.433997460401</v>
+        <v>34477.55246903962</v>
       </c>
       <c r="T20">
-        <v>34197.84586104042</v>
+        <v>34159.10613917779</v>
       </c>
       <c r="U20">
-        <v>33861.305524496718</v>
+        <v>33822.68379622685</v>
       </c>
       <c r="V20">
-        <v>33506.57500378738</v>
+        <v>33468.1480100081</v>
       </c>
       <c r="W20">
-        <v>33147.997440042913</v>
+        <v>33109.9513599721</v>
       </c>
       <c r="X20">
-        <v>32683.299825988772</v>
+        <v>32646.00328544513</v>
       </c>
       <c r="Y20">
-        <v>32169.183204697048</v>
+        <v>32132.77906828077</v>
       </c>
       <c r="Z20">
-        <v>31628.455366061691</v>
+        <v>31592.94415719234</v>
       </c>
       <c r="AA20">
-        <v>31119.432391181021</v>
+        <v>31084.73178071285</v>
       </c>
       <c r="AB20">
-        <v>30691.02146622034</v>
+        <v>30656.95965432574</v>
       </c>
       <c r="AC20">
-        <v>30347.522815020169</v>
+        <v>30313.94309630035</v>
       </c>
       <c r="AD20">
-        <v>30086.043344383019</v>
+        <v>30052.84406512678</v>
       </c>
       <c r="AE20">
-        <v>29880.520534954288</v>
+        <v>29847.74243841253</v>
       </c>
       <c r="AF20">
-        <v>29705.532915951211</v>
+        <v>29673.2569765611</v>
       </c>
       <c r="AG20">
-        <v>29508.432453130161</v>
+        <v>29476.90784570294</v>
       </c>
       <c r="AH20">
-        <v>29194.025573051429</v>
+        <v>29163.53960967701</v>
       </c>
       <c r="AI20">
-        <v>28430.206731181559</v>
+        <v>28401.22930612791</v>
       </c>
       <c r="AJ20">
-        <v>27382.80492351174</v>
+        <v>27355.54075546222</v>
       </c>
       <c r="AK20">
-        <v>26161.722294927851</v>
+        <v>26136.17979349779</v>
       </c>
       <c r="AL20">
-        <v>24970.640337299061</v>
+        <v>24946.63940702065</v>
       </c>
       <c r="AM20">
-        <v>23953.020037936789</v>
+        <v>23930.31723475652</v>
       </c>
       <c r="AN20">
-        <v>23124.872526669511</v>
+        <v>23103.26775437007</v>
       </c>
       <c r="AO20">
-        <v>22420.962389044071</v>
+        <v>22400.3352583318</v>
       </c>
       <c r="AP20">
-        <v>21747.114265946249</v>
+        <v>21727.42041914886</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:42">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>4.5399996391239981</v>
+        <v>4.539999639123998</v>
       </c>
       <c r="D21">
         <v>4.155664675437265</v>
       </c>
       <c r="E21">
-        <v>3.8401416974020601</v>
+        <v>3.84014169740206</v>
       </c>
       <c r="F21">
         <v>3.566986720682134</v>
@@ -2892,40 +2834,40 @@
         <v>3.376883871816323</v>
       </c>
       <c r="H21">
-        <v>3.2310934841529142</v>
+        <v>3.231093484152914</v>
       </c>
       <c r="I21">
-        <v>3.1148411955517288</v>
+        <v>3.114841195551729</v>
       </c>
       <c r="J21">
-        <v>3.0331001301289779</v>
+        <v>3.033100130128978</v>
       </c>
       <c r="K21">
         <v>2.945446165009586</v>
       </c>
       <c r="L21">
-        <v>2.9644827415566959</v>
+        <v>2.964482741556696</v>
       </c>
       <c r="M21">
-        <v>2.9475374507857901</v>
+        <v>2.94753745078579</v>
       </c>
       <c r="N21">
-        <v>2.9639012127436031</v>
+        <v>2.963901212743603</v>
       </c>
       <c r="O21">
-        <v>2.9477828042124119</v>
+        <v>2.947782804212412</v>
       </c>
       <c r="P21">
-        <v>2.9321773943201701</v>
+        <v>2.93217739432017</v>
       </c>
       <c r="Q21">
-        <v>2.8685900878111159</v>
+        <v>2.868590087811116</v>
       </c>
       <c r="R21">
-        <v>2.7805716574304968</v>
+        <v>2.780571657430497</v>
       </c>
       <c r="S21">
-        <v>2.6862074018584661</v>
+        <v>2.686207401858466</v>
       </c>
       <c r="T21">
         <v>2.545077789937944</v>
@@ -2940,16 +2882,16 @@
         <v>2.335326409406842</v>
       </c>
       <c r="X21">
-        <v>2.3344391965778009</v>
+        <v>2.334439196577801</v>
       </c>
       <c r="Y21">
-        <v>2.2405678688925779</v>
+        <v>2.240567868892578</v>
       </c>
       <c r="Z21">
-        <v>2.1250691553982199</v>
+        <v>2.12506915539822</v>
       </c>
       <c r="AA21">
-        <v>1.9676600747376849</v>
+        <v>1.967660074737685</v>
       </c>
       <c r="AB21">
         <v>1.794721712389171</v>
@@ -2970,42 +2912,42 @@
         <v>1.303106783029345</v>
       </c>
       <c r="AH21">
-        <v>1.2918047226972109</v>
+        <v>1.291804722697211</v>
       </c>
       <c r="AI21">
-        <v>1.3910440226302481</v>
+        <v>1.391044022630248</v>
       </c>
       <c r="AJ21">
-        <v>1.3879417857775711</v>
+        <v>1.387941785777571</v>
       </c>
       <c r="AK21">
         <v>1.327516434160759</v>
       </c>
       <c r="AL21">
-        <v>1.1965330624649699</v>
+        <v>1.19653306246497</v>
       </c>
       <c r="AM21">
-        <v>1.0353571648568101</v>
+        <v>1.03535716485681</v>
       </c>
       <c r="AN21">
-        <v>0.89313654931279896</v>
+        <v>0.893136549312799</v>
       </c>
       <c r="AO21">
-        <v>0.78811942926007916</v>
+        <v>0.7881194292600792</v>
       </c>
       <c r="AP21">
-        <v>0.71915415589639187</v>
+        <v>0.7191541558963919</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:42">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.43821573912399819</v>
+        <v>0.4382157391239982</v>
       </c>
       <c r="D22">
         <v>0.4434740194859122</v>
@@ -3014,85 +2956,85 @@
         <v>0.4506175604103293</v>
       </c>
       <c r="F22">
-        <v>0.45946169865589909</v>
+        <v>0.4594616986558991</v>
       </c>
       <c r="G22">
-        <v>0.46964065541714078</v>
+        <v>0.4696406554171408</v>
       </c>
       <c r="H22">
-        <v>0.48045848753949078</v>
+        <v>0.4804584875394908</v>
       </c>
       <c r="I22">
-        <v>0.49158630685099741</v>
+        <v>0.4915863068509974</v>
       </c>
       <c r="J22">
-        <v>0.50294027272380648</v>
+        <v>0.5029402727238065</v>
       </c>
       <c r="K22">
-        <v>0.51415643301265423</v>
+        <v>0.5141564330126542</v>
       </c>
       <c r="L22">
         <v>0.5245848586137497</v>
       </c>
       <c r="M22">
-        <v>0.53407316274241989</v>
+        <v>0.5340731627424199</v>
       </c>
       <c r="N22">
-        <v>0.54207738327408017</v>
+        <v>0.5420773832740802</v>
       </c>
       <c r="O22">
-        <v>0.54881275076858482</v>
+        <v>0.5488127507685848</v>
       </c>
       <c r="P22">
-        <v>0.55415486274119674</v>
+        <v>0.5541548627411967</v>
       </c>
       <c r="Q22">
-        <v>0.55854626868095458</v>
+        <v>0.5585462686809546</v>
       </c>
       <c r="R22">
-        <v>0.56213595593093113</v>
+        <v>0.5621359559309311</v>
       </c>
       <c r="S22">
-        <v>0.56475085608705744</v>
+        <v>0.5647508560870574</v>
       </c>
       <c r="T22">
-        <v>0.56690638302054053</v>
+        <v>0.5669063830205405</v>
       </c>
       <c r="U22">
         <v>0.5682083534918797</v>
       </c>
       <c r="V22">
-        <v>0.56832928081473921</v>
+        <v>0.5683292808147392</v>
       </c>
       <c r="W22">
         <v>0.5664798733263785</v>
       </c>
       <c r="X22">
-        <v>0.56180824046984335</v>
+        <v>0.5618082404698433</v>
       </c>
       <c r="Y22">
         <v>0.5541424924548688</v>
       </c>
       <c r="Z22">
-        <v>0.54328454638406209</v>
+        <v>0.5432845463840621</v>
       </c>
       <c r="AA22">
-        <v>0.52980771640863311</v>
+        <v>0.5298077164086331</v>
       </c>
       <c r="AB22">
-        <v>0.51400447480866807</v>
+        <v>0.5140044748086681</v>
       </c>
       <c r="AC22">
         <v>0.4959738957039615</v>
       </c>
       <c r="AD22">
-        <v>0.47590605578056983</v>
+        <v>0.4759060557805698</v>
       </c>
       <c r="AE22">
-        <v>0.45411004229428642</v>
+        <v>0.4541100422942864</v>
       </c>
       <c r="AF22">
-        <v>0.43114023589102962</v>
+        <v>0.4311402358910296</v>
       </c>
       <c r="AG22">
         <v>0.4077410773653104</v>
@@ -3101,32 +3043,32 @@
         <v>0.3842994570778987</v>
       </c>
       <c r="AI22">
-        <v>0.36082284441734169</v>
+        <v>0.3608228444173417</v>
       </c>
       <c r="AJ22">
-        <v>0.33802636458707419</v>
+        <v>0.3380263645870742</v>
       </c>
       <c r="AK22">
-        <v>0.31655694146412439</v>
+        <v>0.3165569414641244</v>
       </c>
       <c r="AL22">
         <v>0.2971878449900886</v>
       </c>
       <c r="AM22">
-        <v>0.28022712387053522</v>
+        <v>0.2802271238705352</v>
       </c>
       <c r="AN22">
-        <v>0.26562566331407672</v>
+        <v>0.2656256633140767</v>
       </c>
       <c r="AO22">
-        <v>0.25323787947883369</v>
+        <v>0.2532378794788337</v>
       </c>
       <c r="AP22">
-        <v>0.24260568363508159</v>
+        <v>0.2426056836350816</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:42">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -3253,21 +3195,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:42">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>4.1017838999999983</v>
+        <v>4.101783899999998</v>
       </c>
       <c r="D24">
-        <v>3.7121906559513458</v>
+        <v>3.712190655951346</v>
       </c>
       <c r="E24">
-        <v>3.3895241369917239</v>
+        <v>3.389524136991724</v>
       </c>
       <c r="F24">
         <v>3.10752502202623</v>
@@ -3282,46 +3224,46 @@
         <v>2.623254888700727</v>
       </c>
       <c r="J24">
-        <v>2.5301598574051658</v>
+        <v>2.530159857405166</v>
       </c>
       <c r="K24">
-        <v>2.4312897319969249</v>
+        <v>2.431289731996925</v>
       </c>
       <c r="L24">
-        <v>2.4398978829429421</v>
+        <v>2.439897882942942</v>
       </c>
       <c r="M24">
-        <v>2.4134642880433659</v>
+        <v>2.413464288043366</v>
       </c>
       <c r="N24">
-        <v>2.4218238294695191</v>
+        <v>2.421823829469519</v>
       </c>
       <c r="O24">
-        <v>2.3989700534438239</v>
+        <v>2.398970053443824</v>
       </c>
       <c r="P24">
         <v>2.378022531578968</v>
       </c>
       <c r="Q24">
-        <v>2.3100438191301582</v>
+        <v>2.310043819130158</v>
       </c>
       <c r="R24">
         <v>2.218435701499561</v>
       </c>
       <c r="S24">
-        <v>2.1214565457714021</v>
+        <v>2.121456545771402</v>
       </c>
       <c r="T24">
-        <v>1.9781714069173979</v>
+        <v>1.978171406917398</v>
       </c>
       <c r="U24">
-        <v>1.8707237074886089</v>
+        <v>1.870723707488609</v>
       </c>
       <c r="V24">
         <v>1.829119026740871</v>
       </c>
       <c r="W24">
-        <v>1.7688465360804571</v>
+        <v>1.768846536080457</v>
       </c>
       <c r="X24">
         <v>1.772630956107953</v>
@@ -3330,34 +3272,34 @@
         <v>1.686425376437704</v>
       </c>
       <c r="Z24">
-        <v>1.5817846090141521</v>
+        <v>1.581784609014152</v>
       </c>
       <c r="AA24">
-        <v>1.4378523583290459</v>
+        <v>1.437852358329046</v>
       </c>
       <c r="AB24">
-        <v>1.2807172375804969</v>
+        <v>1.280717237580497</v>
       </c>
       <c r="AC24">
-        <v>1.1604287487937619</v>
+        <v>1.160428748793762</v>
       </c>
       <c r="AD24">
-        <v>1.0507863395765329</v>
+        <v>1.050786339576533</v>
       </c>
       <c r="AE24">
-        <v>0.97347279427033584</v>
+        <v>0.9734727942703358</v>
       </c>
       <c r="AF24">
-        <v>0.92663107881026596</v>
+        <v>0.926631078810266</v>
       </c>
       <c r="AG24">
         <v>0.8953657056640294</v>
       </c>
       <c r="AH24">
-        <v>0.90750526561930589</v>
+        <v>0.9075052656193059</v>
       </c>
       <c r="AI24">
-        <v>1.0302211782129009</v>
+        <v>1.030221178212901</v>
       </c>
       <c r="AJ24">
         <v>1.049915421190492</v>
@@ -3369,93 +3311,93 @@
         <v>0.8993452174748755</v>
       </c>
       <c r="AM24">
-        <v>0.75513004098627001</v>
+        <v>0.75513004098627</v>
       </c>
       <c r="AN24">
-        <v>0.62751088599871652</v>
+        <v>0.6275108859987165</v>
       </c>
       <c r="AO24">
-        <v>0.53488154978123992</v>
+        <v>0.5348815497812399</v>
       </c>
       <c r="AP24">
-        <v>0.47654847226130698</v>
+        <v>0.476548472261307</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:42">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
       <c r="C25">
-        <v>95.460000360875995</v>
+        <v>95.46000036087599</v>
       </c>
       <c r="D25">
         <v>91.30433568543873</v>
       </c>
       <c r="E25">
-        <v>87.464193988036669</v>
+        <v>87.46419398803667</v>
       </c>
       <c r="F25">
-        <v>83.897207267354531</v>
+        <v>83.89720726735453</v>
       </c>
       <c r="G25">
-        <v>80.520323395538199</v>
+        <v>80.5203233955382</v>
       </c>
       <c r="H25">
-        <v>77.289229911385277</v>
+        <v>77.28922991138528</v>
       </c>
       <c r="I25">
-        <v>74.174388715833544</v>
+        <v>74.17438871583354</v>
       </c>
       <c r="J25">
-        <v>71.141288585704558</v>
+        <v>71.14128858570456</v>
       </c>
       <c r="K25">
-        <v>68.195842420694973</v>
+        <v>68.19584242069497</v>
       </c>
       <c r="L25">
-        <v>65.231359679138279</v>
+        <v>65.23135967913828</v>
       </c>
       <c r="M25">
-        <v>62.283822228352477</v>
+        <v>62.28382222835248</v>
       </c>
       <c r="N25">
         <v>59.31992101560887</v>
       </c>
       <c r="O25">
-        <v>56.372138211396447</v>
+        <v>56.37213821139645</v>
       </c>
       <c r="P25">
-        <v>53.439960817076283</v>
+        <v>53.43996081707628</v>
       </c>
       <c r="Q25">
-        <v>50.571370729265148</v>
+        <v>50.57137072926515</v>
       </c>
       <c r="R25">
-        <v>47.790799071834662</v>
+        <v>47.79079907183466</v>
       </c>
       <c r="S25">
         <v>45.10459166997618</v>
       </c>
       <c r="T25">
-        <v>42.559513880038232</v>
+        <v>42.55951388003823</v>
       </c>
       <c r="U25">
-        <v>40.120581819057733</v>
+        <v>40.12058181905773</v>
       </c>
       <c r="V25">
         <v>37.72313351150212</v>
       </c>
       <c r="W25">
-        <v>35.387807102095273</v>
+        <v>35.38780710209527</v>
       </c>
       <c r="X25">
-        <v>33.053367905517462</v>
+        <v>33.05336790551746</v>
       </c>
       <c r="Y25">
-        <v>30.812800036624878</v>
+        <v>30.81280003662488</v>
       </c>
       <c r="Z25">
         <v>28.68773088122666</v>
@@ -3467,10 +3409,10 @@
         <v>24.92534909409979</v>
       </c>
       <c r="AC25">
-        <v>23.268946449602058</v>
+        <v>23.26894644960206</v>
       </c>
       <c r="AD25">
-        <v>21.742254054244949</v>
+        <v>21.74225405424495</v>
       </c>
       <c r="AE25">
         <v>20.31467121768031</v>
@@ -3479,38 +3421,38 @@
         <v>18.956899902979</v>
       </c>
       <c r="AG25">
-        <v>17.653793119949661</v>
+        <v>17.65379311994966</v>
       </c>
       <c r="AH25">
-        <v>16.361988397252439</v>
+        <v>16.36198839725244</v>
       </c>
       <c r="AI25">
         <v>14.97094437462219</v>
       </c>
       <c r="AJ25">
-        <v>13.583002588844611</v>
+        <v>13.58300258884461</v>
       </c>
       <c r="AK25">
-        <v>12.255486154683849</v>
+        <v>12.25548615468385</v>
       </c>
       <c r="AL25">
         <v>11.05895309221888</v>
       </c>
       <c r="AM25">
-        <v>10.023595927362059</v>
+        <v>10.02359592736206</v>
       </c>
       <c r="AN25">
         <v>9.130459378049256</v>
       </c>
       <c r="AO25">
-        <v>8.3423399487891707</v>
+        <v>8.342339948789171</v>
       </c>
       <c r="AP25">
-        <v>7.6231857928927749</v>
+        <v>7.623185792892775</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:42">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26">
@@ -3520,249 +3462,505 @@
         <v>14199883.24327</v>
       </c>
       <c r="D26">
-        <v>14111151.03168831</v>
+        <v>14109177.79601758</v>
       </c>
       <c r="E26">
-        <v>14064028.516302601</v>
+        <v>14060187.24711843</v>
       </c>
       <c r="F26">
-        <v>14049664.32730386</v>
+        <v>14044054.71679426</v>
       </c>
       <c r="G26">
-        <v>14061382.740197361</v>
+        <v>14054096.69691078</v>
       </c>
       <c r="H26">
-        <v>14087265.980035471</v>
+        <v>14078386.7250649</v>
       </c>
       <c r="I26">
-        <v>14118751.800130431</v>
+        <v>14108363.43802984</v>
       </c>
       <c r="J26">
-        <v>14148641.192651501</v>
+        <v>14136816.4563964</v>
       </c>
       <c r="K26">
-        <v>14167132.11985884</v>
+        <v>14154980.87897542</v>
       </c>
       <c r="L26">
-        <v>14181308.33923416</v>
+        <v>14168833.33664557</v>
       </c>
       <c r="M26">
-        <v>14183371.292032329</v>
+        <v>14170585.72855761</v>
       </c>
       <c r="N26">
-        <v>14176848.666921159</v>
+        <v>14163781.38435228</v>
       </c>
       <c r="O26">
-        <v>14156121.64789591</v>
+        <v>14142830.15064871</v>
       </c>
       <c r="P26">
-        <v>14115940.952702969</v>
+        <v>14102471.42015605</v>
       </c>
       <c r="Q26">
-        <v>14037234.280246601</v>
+        <v>14023652.22068979</v>
       </c>
       <c r="R26">
-        <v>13923106.729342081</v>
+        <v>13909487.11410913</v>
       </c>
       <c r="S26">
-        <v>13769406.983990731</v>
+        <v>13755784.16643228</v>
       </c>
       <c r="T26">
-        <v>13585521.244889161</v>
+        <v>13571898.48064623</v>
       </c>
       <c r="U26">
-        <v>13396397.811397269</v>
+        <v>13382754.09864111</v>
       </c>
       <c r="V26">
-        <v>13202831.95521467</v>
+        <v>13189158.53710954</v>
       </c>
       <c r="W26">
-        <v>12995020.585179459</v>
+        <v>12981344.61650524</v>
       </c>
       <c r="X26">
-        <v>12774977.035298539</v>
+        <v>12761356.88448417</v>
       </c>
       <c r="Y26">
-        <v>12507421.335295171</v>
+        <v>12493962.29478219</v>
       </c>
       <c r="Z26">
-        <v>12221630.040321181</v>
+        <v>12208386.55134734</v>
       </c>
       <c r="AA26">
-        <v>11932549.464707229</v>
+        <v>11919535.63849512</v>
       </c>
       <c r="AB26">
-        <v>11661508.92328639</v>
+        <v>11648705.59068756</v>
       </c>
       <c r="AC26">
-        <v>11424906.771819251</v>
+        <v>11412269.12588785</v>
       </c>
       <c r="AD26">
-        <v>11220114.59842086</v>
+        <v>11207604.21158734</v>
       </c>
       <c r="AE26">
-        <v>11043512.97347321</v>
+        <v>11031110.0490581</v>
       </c>
       <c r="AF26">
-        <v>10881705.553554781</v>
+        <v>10869439.89008718</v>
       </c>
       <c r="AG26">
-        <v>10726278.26694216</v>
+        <v>10714187.16778584</v>
       </c>
       <c r="AH26">
-        <v>10561109.74978698</v>
+        <v>10549255.18111337</v>
       </c>
       <c r="AI26">
-        <v>10354968.81611553</v>
+        <v>10343415.12557808</v>
       </c>
       <c r="AJ26">
-        <v>10007692.53014956</v>
+        <v>9996574.772915</v>
       </c>
       <c r="AK26">
-        <v>9576943.9886050262</v>
+        <v>9566329.898440944</v>
       </c>
       <c r="AL26">
-        <v>9100871.3294437733</v>
+        <v>9090785.46788137</v>
       </c>
       <c r="AM26">
-        <v>8644567.5236459747</v>
+        <v>8634979.557898201</v>
       </c>
       <c r="AN26">
-        <v>8251442.598735786</v>
+        <v>8242292.393502236</v>
       </c>
       <c r="AO26">
-        <v>7923994.6897185622</v>
+        <v>7915225.021370769</v>
       </c>
       <c r="AP26">
-        <v>7640264.3480006568</v>
+        <v>7631837.572410492</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:42">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>14199883.24327</v>
       </c>
       <c r="C27">
-        <v>14111151.03168831</v>
+        <v>14109177.79601758</v>
       </c>
       <c r="D27">
-        <v>14064028.516302601</v>
+        <v>14060187.24711843</v>
       </c>
       <c r="E27">
-        <v>14049664.32730386</v>
+        <v>14044054.71679426</v>
       </c>
       <c r="F27">
-        <v>14061382.740197361</v>
+        <v>14054096.69691078</v>
       </c>
       <c r="G27">
-        <v>14087265.980035471</v>
+        <v>14078386.7250649</v>
       </c>
       <c r="H27">
-        <v>14118751.800130431</v>
+        <v>14108363.43802984</v>
       </c>
       <c r="I27">
-        <v>14148641.192651501</v>
+        <v>14136816.4563964</v>
       </c>
       <c r="J27">
-        <v>14167132.11985884</v>
+        <v>14154980.87897542</v>
       </c>
       <c r="K27">
-        <v>14181308.33923416</v>
+        <v>14168833.33664557</v>
       </c>
       <c r="L27">
-        <v>14183371.292032329</v>
+        <v>14170585.72855761</v>
       </c>
       <c r="M27">
-        <v>14176848.666921159</v>
+        <v>14163781.38435228</v>
       </c>
       <c r="N27">
-        <v>14156121.64789591</v>
+        <v>14142830.15064871</v>
       </c>
       <c r="O27">
-        <v>14115940.952702969</v>
+        <v>14102471.42015605</v>
       </c>
       <c r="P27">
-        <v>14037234.280246601</v>
+        <v>14023652.22068979</v>
       </c>
       <c r="Q27">
-        <v>13923106.729342081</v>
+        <v>13909487.11410913</v>
       </c>
       <c r="R27">
-        <v>13769406.983990731</v>
+        <v>13755784.16643228</v>
       </c>
       <c r="S27">
-        <v>13585521.244889161</v>
+        <v>13571898.48064623</v>
       </c>
       <c r="T27">
-        <v>13396397.811397269</v>
+        <v>13382754.09864111</v>
       </c>
       <c r="U27">
-        <v>13202831.95521467</v>
+        <v>13189158.53710954</v>
       </c>
       <c r="V27">
-        <v>12995020.585179459</v>
+        <v>12981344.61650524</v>
       </c>
       <c r="W27">
-        <v>12774977.035298539</v>
+        <v>12761356.88448417</v>
       </c>
       <c r="X27">
-        <v>12507421.335295171</v>
+        <v>12493962.29478219</v>
       </c>
       <c r="Y27">
-        <v>12221630.040321181</v>
+        <v>12208386.55134734</v>
       </c>
       <c r="Z27">
-        <v>11932549.464707229</v>
+        <v>11919535.63849512</v>
       </c>
       <c r="AA27">
-        <v>11661508.92328639</v>
+        <v>11648705.59068756</v>
       </c>
       <c r="AB27">
-        <v>11424906.771819251</v>
+        <v>11412269.12588785</v>
       </c>
       <c r="AC27">
-        <v>11220114.59842086</v>
+        <v>11207604.21158734</v>
       </c>
       <c r="AD27">
-        <v>11043512.97347321</v>
+        <v>11031110.0490581</v>
       </c>
       <c r="AE27">
-        <v>10881705.553554781</v>
+        <v>10869439.89008718</v>
       </c>
       <c r="AF27">
-        <v>10726278.26694216</v>
+        <v>10714187.16778584</v>
       </c>
       <c r="AG27">
-        <v>10561109.74978698</v>
+        <v>10549255.18111337</v>
       </c>
       <c r="AH27">
-        <v>10354968.81611553</v>
+        <v>10343415.12557808</v>
       </c>
       <c r="AI27">
-        <v>10007692.53014956</v>
+        <v>9996574.772915</v>
       </c>
       <c r="AJ27">
-        <v>9576943.9886050262</v>
+        <v>9566329.898440944</v>
       </c>
       <c r="AK27">
-        <v>9100871.3294437733</v>
+        <v>9090785.46788137</v>
       </c>
       <c r="AL27">
-        <v>8644567.5236459747</v>
+        <v>8634979.557898201</v>
       </c>
       <c r="AM27">
-        <v>8251442.598735786</v>
+        <v>8242292.393502236</v>
       </c>
       <c r="AN27">
-        <v>7923994.6897185622</v>
+        <v>7915225.021370769</v>
       </c>
       <c r="AO27">
-        <v>7640264.3480006568</v>
+        <v>7631837.572410492</v>
       </c>
       <c r="AP27">
-        <v>7369932.8182373242</v>
+        <v>7361836.466397768</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>-618053.5179209257</v>
+      </c>
+      <c r="D28">
+        <v>-619624.656720613</v>
+      </c>
+      <c r="E28">
+        <v>-623165.8236664238</v>
+      </c>
+      <c r="F28">
+        <v>-628316.1349636839</v>
+      </c>
+      <c r="G28">
+        <v>-634515.7734301449</v>
+      </c>
+      <c r="H28">
+        <v>-641219.7368372924</v>
+      </c>
+      <c r="I28">
+        <v>-647954.9689466307</v>
+      </c>
+      <c r="J28">
+        <v>-654175.4185074128</v>
+      </c>
+      <c r="K28">
+        <v>-659837.3041755706</v>
+      </c>
+      <c r="L28">
+        <v>-665049.0515153974</v>
+      </c>
+      <c r="M28">
+        <v>-669856.2867147655</v>
+      </c>
+      <c r="N28">
+        <v>-674484.5044178888</v>
+      </c>
+      <c r="O28">
+        <v>-678666.7835146192</v>
+      </c>
+      <c r="P28">
+        <v>-681609.6726672727</v>
+      </c>
+      <c r="Q28">
+        <v>-682716.7158071124</v>
+      </c>
+      <c r="R28">
+        <v>-681469.698523415</v>
+      </c>
+      <c r="S28">
+        <v>-677554.2085204842</v>
+      </c>
+      <c r="T28">
+        <v>-671902.3540106594</v>
+      </c>
+      <c r="U28">
+        <v>-665584.2302205012</v>
+      </c>
+      <c r="V28">
+        <v>-658912.6767155542</v>
+      </c>
+      <c r="W28">
+        <v>-652033.6068088309</v>
+      </c>
+      <c r="X28">
+        <v>-644186.9284366677</v>
+      </c>
+      <c r="Y28">
+        <v>-634792.8182831048</v>
+      </c>
+      <c r="Z28">
+        <v>-624637.3511955542</v>
+      </c>
+      <c r="AA28">
+        <v>-614471.9426243153</v>
+      </c>
+      <c r="AB28">
+        <v>-605353.8863900009</v>
+      </c>
+      <c r="AC28">
+        <v>-597843.7526952975</v>
+      </c>
+      <c r="AD28">
+        <v>-591970.1829078449</v>
+      </c>
+      <c r="AE28">
+        <v>-587476.4717662121</v>
+      </c>
+      <c r="AF28">
+        <v>-583863.6275693695</v>
+      </c>
+      <c r="AG28">
+        <v>-580386.1599678509</v>
+      </c>
+      <c r="AH28">
+        <v>-575625.6232292933</v>
+      </c>
+      <c r="AI28">
+        <v>-565588.3812468317</v>
+      </c>
+      <c r="AJ28">
+        <v>-548196.8356104246</v>
+      </c>
+      <c r="AK28">
+        <v>-526201.9768065183</v>
+      </c>
+      <c r="AL28">
+        <v>-502600.1482486462</v>
+      </c>
+      <c r="AM28">
+        <v>-480856.7563417114</v>
+      </c>
+      <c r="AN28">
+        <v>-462654.8467958642</v>
+      </c>
+      <c r="AO28">
+        <v>-447585.5640598492</v>
+      </c>
+      <c r="AP28">
+        <v>-434108.245276942</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>-14817936.76119093</v>
+      </c>
+      <c r="D29">
+        <v>-14728802.45273819</v>
+      </c>
+      <c r="E29">
+        <v>-14683353.07078486</v>
+      </c>
+      <c r="F29">
+        <v>-14672370.85175795</v>
+      </c>
+      <c r="G29">
+        <v>-14688612.47034092</v>
+      </c>
+      <c r="H29">
+        <v>-14719606.4619022</v>
+      </c>
+      <c r="I29">
+        <v>-14756318.40697647</v>
+      </c>
+      <c r="J29">
+        <v>-14792038.79181228</v>
+      </c>
+      <c r="K29">
+        <v>-14815829.5419796</v>
+      </c>
+      <c r="L29">
+        <v>-14834859.372261</v>
+      </c>
+      <c r="M29">
+        <v>-14841382.67891238</v>
+      </c>
+      <c r="N29">
+        <v>-14839165.29298628</v>
+      </c>
+      <c r="O29">
+        <v>-14822354.18579696</v>
+      </c>
+      <c r="P29">
+        <v>-14784896.49582371</v>
+      </c>
+      <c r="Q29">
+        <v>-14707140.50071597</v>
+      </c>
+      <c r="R29">
+        <v>-14591688.06838009</v>
+      </c>
+      <c r="S29">
+        <v>-14434035.01145015</v>
+      </c>
+      <c r="T29">
+        <v>-14244468.78699671</v>
+      </c>
+      <c r="U29">
+        <v>-14048982.4431886</v>
+      </c>
+      <c r="V29">
+        <v>-13848690.64454365</v>
+      </c>
+      <c r="W29">
+        <v>-13633969.3555625</v>
+      </c>
+      <c r="X29">
+        <v>-13406100.98678509</v>
+      </c>
+      <c r="Y29">
+        <v>-13129277.41570706</v>
+      </c>
+      <c r="Z29">
+        <v>-12833514.07689133</v>
+      </c>
+      <c r="AA29">
+        <v>-12534469.95279517</v>
+      </c>
+      <c r="AB29">
+        <v>-12254498.75506059</v>
+      </c>
+      <c r="AC29">
+        <v>-12010532.20271931</v>
+      </c>
+      <c r="AD29">
+        <v>-11799974.64723011</v>
+      </c>
+      <c r="AE29">
+        <v>-11618962.77719237</v>
+      </c>
+      <c r="AF29">
+        <v>-11453652.41571201</v>
+      </c>
+      <c r="AG29">
+        <v>-11294893.44207914</v>
+      </c>
+      <c r="AH29">
+        <v>-11125173.99527679</v>
+      </c>
+      <c r="AI29">
+        <v>-10909269.44483144</v>
+      </c>
+      <c r="AJ29">
+        <v>-10545012.08359726</v>
+      </c>
+      <c r="AK29">
+        <v>-10092749.02233749</v>
+      </c>
+      <c r="AL29">
+        <v>-9593582.074218003</v>
+      </c>
+      <c r="AM29">
+        <v>-9116014.786138607</v>
+      </c>
+      <c r="AN29">
+        <v>-8705110.056660032</v>
+      </c>
+      <c r="AO29">
+        <v>-8362959.727608008</v>
+      </c>
+      <c r="AP29">
+        <v>-8066082.78871685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>